<commit_message>
new xlsx with line size changed to line width
</commit_message>
<xml_diff>
--- a/quizzes/ls01_gg_intro/ls01_gg_intro_theory_quiz/quiz.xlsx
+++ b/quizzes/ls01_gg_intro/ls01_gg_intro_theory_quiz/quiz.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:W18"/>
+  <dimension ref="A1:W19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -505,22 +505,30 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>Graphical geometries</t>
+          <t>&lt;div id="a" class="section level2"&gt;_x000D_
+&lt;h2&gt;A&lt;/h2&gt;_x000D_
+&lt;p&gt;Graphical geometries&lt;/p&gt;_x000D_&lt;/div&gt;</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>Grey goose</t>
+          <t>&lt;div id="b" class="section level2"&gt;_x000D_
+&lt;h2&gt;B&lt;/h2&gt;_x000D_
+&lt;p&gt;Grey goose&lt;/p&gt;_x000D_&lt;/div&gt;</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>Grammar of graphics</t>
+          <t>&lt;div id="c" class="section level2"&gt;_x000D_
+&lt;h2&gt;C&lt;/h2&gt;_x000D_
+&lt;p&gt;Grammar of graphics&lt;/p&gt;_x000D_&lt;/div&gt;</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>Good game</t>
+          <t>&lt;div id="d" class="section level2"&gt;_x000D_
+&lt;h2&gt;D&lt;/h2&gt;_x000D_
+&lt;p&gt;Good game&lt;/p&gt;_x000D_&lt;/div&gt;</t>
         </is>
       </c>
       <c r="T2">
@@ -528,14 +536,16 @@
       </c>
       <c r="U2" t="inlineStr">
         <is>
-          <t>Good game!
-GG stands for &lt;strong&gt;G&lt;/strong&gt;rammar of &lt;strong&gt;G&lt;/strong&gt;raphics.</t>
+          <t>&lt;div id="correct-message" class="section level2"&gt;_x000D_
+&lt;h2&gt;Correct message&lt;/h2&gt;_x000D_
+&lt;p&gt;Good game! GG stands for &lt;strong&gt;G&lt;/strong&gt;rammar of &lt;strong&gt;G&lt;/strong&gt;raphics.&lt;/p&gt;_x000D_&lt;/div&gt;</t>
         </is>
       </c>
       <c r="V2" t="inlineStr">
         <is>
-          <t>Nice try, but not this time.
-GG stands for &lt;strong&gt;G&lt;/strong&gt;rammar of &lt;strong&gt;G&lt;/strong&gt;raphics.</t>
+          <t>&lt;div id="incorrect-message" class="section level2"&gt;_x000D_
+&lt;h2&gt;Incorrect message&lt;/h2&gt;_x000D_
+&lt;p&gt;Nice try, but not this time. GG stands for &lt;strong&gt;G&lt;/strong&gt;rammar of &lt;strong&gt;G&lt;/strong&gt;raphics.&lt;/p&gt;_x000D_&lt;/div&gt;</t>
         </is>
       </c>
     </row>
@@ -560,22 +570,30 @@
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>{base}</t>
+          <t>&lt;div id="a-1" class="section level2"&gt;_x000D_
+&lt;h2&gt;A&lt;/h2&gt;_x000D_
+&lt;p&gt;{base}&lt;/p&gt;_x000D_&lt;/div&gt;</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>{ggplot}</t>
+          <t>&lt;div id="b-1" class="section level2"&gt;_x000D_
+&lt;h2&gt;B&lt;/h2&gt;_x000D_
+&lt;p&gt;{ggplot}&lt;/p&gt;_x000D_&lt;/div&gt;</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>{tidyverse}</t>
+          <t>&lt;div id="c-1" class="section level2"&gt;_x000D_
+&lt;h2&gt;C&lt;/h2&gt;_x000D_
+&lt;p&gt;{tidyverse}&lt;/p&gt;_x000D_&lt;/div&gt;</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>{ggplot2}</t>
+          <t>&lt;div id="d-1" class="section level2"&gt;_x000D_
+&lt;h2&gt;D&lt;/h2&gt;_x000D_
+&lt;p&gt;{ggplot2}&lt;/p&gt;_x000D_&lt;/div&gt;</t>
         </is>
       </c>
       <c r="T3">
@@ -583,12 +601,16 @@
       </c>
       <c r="U3" t="inlineStr">
         <is>
-          <t>You remembered! We use {ggplot2} for this course.</t>
+          <t>&lt;div id="correct-message-1" class="section level2"&gt;_x000D_
+&lt;h2&gt;Correct message&lt;/h2&gt;_x000D_
+&lt;p&gt;You remembered! We use {ggplot2} for this course.&lt;/p&gt;_x000D_&lt;/div&gt;</t>
         </is>
       </c>
       <c r="V3" t="inlineStr">
         <is>
-          <t>Sorry, that’s not it. If you go back to the lessons, or some of the Esquisser graphs we’ve made, you’ll see we use {ggplot2}.</t>
+          <t>&lt;div id="incorrect-message-1" class="section level2"&gt;_x000D_
+&lt;h2&gt;Incorrect message&lt;/h2&gt;_x000D_
+&lt;p&gt;Sorry, that’s not it. If you go back to the lessons, or some of the Esquisser graphs we’ve made, you’ll see we use {ggplot2}.&lt;/p&gt;_x000D_&lt;/div&gt;</t>
         </is>
       </c>
     </row>
@@ -613,12 +635,16 @@
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>FALSE</t>
+          <t>&lt;div id="a-2" class="section level2"&gt;_x000D_
+&lt;h2&gt;A&lt;/h2&gt;_x000D_
+&lt;p&gt;FALSE&lt;/p&gt;_x000D_&lt;/div&gt;</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>TRUE</t>
+          <t>&lt;div id="b-2" class="section level2"&gt;_x000D_
+&lt;h2&gt;B&lt;/h2&gt;_x000D_
+&lt;p&gt;TRUE&lt;/p&gt;_x000D_&lt;/div&gt;</t>
         </is>
       </c>
       <c r="T4">
@@ -626,12 +652,16 @@
       </c>
       <c r="U4" t="inlineStr">
         <is>
-          <t>Indeed, {ggplot2} is a core tidyverse package. You can take a look at the &lt;a href="https://www.tidyverse.org/" target="_blank"&gt;tidyverse website&lt;/a&gt; to see all the packages in the tidyverse.</t>
+          <t>&lt;div id="correct-message-2" class="section level2"&gt;_x000D_
+&lt;h2&gt;Correct message&lt;/h2&gt;_x000D_
+&lt;p&gt;Indeed, {ggplot2} is a core tidyverse package. You can take a look at the &lt;a href="https://www.tidyverse.org/" target="_blank"&gt;tidyverse website&lt;/a&gt; to see all the packages in the tidyverse.&lt;/p&gt;_x000D_&lt;/div&gt;</t>
         </is>
       </c>
       <c r="V4" t="inlineStr">
         <is>
-          <t>{ggplot2} is a core tidyverse package. You can take a look at the &lt;a href="https://www.tidyverse.org/" target="_blank"&gt;tidyverse website&lt;/a&gt; to see all the packages in the tidyverse.</t>
+          <t>&lt;div id="incorrect-message-2" class="section level2"&gt;_x000D_
+&lt;h2&gt;Incorrect message&lt;/h2&gt;_x000D_
+&lt;p&gt;{ggplot2} is a core tidyverse package. You can take a look at the &lt;a href="https://www.tidyverse.org/" target="_blank"&gt;tidyverse website&lt;/a&gt; to see all the packages in the tidyverse.&lt;/p&gt;_x000D_&lt;/div&gt;</t>
         </is>
       </c>
     </row>
@@ -656,17 +686,23 @@
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>&lt;code&gt;library(tidyverse)&lt;/code&gt;</t>
+          <t>&lt;div id="a-3" class="section level2"&gt;_x000D_
+&lt;h2&gt;A&lt;/h2&gt;_x000D_
+&lt;p&gt;&lt;code&gt;library(tidyverse)&lt;/code&gt;&lt;/p&gt;_x000D_&lt;/div&gt;</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>&lt;code&gt;library(ggplot)&lt;/code&gt;</t>
+          <t>&lt;div id="b-3" class="section level2"&gt;_x000D_
+&lt;h2&gt;B&lt;/h2&gt;_x000D_
+&lt;p&gt;&lt;code&gt;library(ggplot)&lt;/code&gt;&lt;/p&gt;_x000D_&lt;/div&gt;</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>&lt;code&gt;library(ggplot2)&lt;/code&gt;</t>
+          <t>&lt;div id="c-2" class="section level2"&gt;_x000D_
+&lt;h2&gt;C&lt;/h2&gt;_x000D_
+&lt;p&gt;&lt;code&gt;library(ggplot2)&lt;/code&gt;&lt;/p&gt;_x000D_&lt;/div&gt;</t>
         </is>
       </c>
       <c r="T5">
@@ -674,14 +710,18 @@
       </c>
       <c r="U5" t="inlineStr">
         <is>
-          <t>Nice one! Loading either {ggplot2} or {tidyverse} (which includes {ggplot2}) get us {ggplot2}.&lt;/p&gt;
-&lt;p&gt;It can be confusing, but remember that {ggplot2} is the package and &lt;code&gt;ggplot()&lt;/code&gt; is the key function in that package.</t>
+          <t>&lt;div id="correct-message-3" class="section level2"&gt;_x000D_
+&lt;h2&gt;Correct message&lt;/h2&gt;_x000D_
+&lt;p&gt;Nice one! Loading either {ggplot2} or {tidyverse} (which includes {ggplot2}) get us {ggplot2}.&lt;/p&gt;_x000D_
+&lt;p&gt;It can be confusing, but remember that {ggplot2} is the package and &lt;code&gt;ggplot()&lt;/code&gt; is the key function in that package.&lt;/p&gt;_x000D_&lt;/div&gt;</t>
         </is>
       </c>
       <c r="V5" t="inlineStr">
         <is>
-          <t>Loading either {ggplot2} or {tidyverse} (which includes {ggplot2}) get us {ggplot2}.&lt;/p&gt;
-&lt;p&gt;It can be confusing, but remember that {ggplot2} is the package and &lt;code&gt;ggplot()&lt;/code&gt; is the key function in that package.</t>
+          <t>&lt;div id="incorrect-message-3" class="section level2"&gt;_x000D_
+&lt;h2&gt;Incorrect message&lt;/h2&gt;_x000D_
+&lt;p&gt;Loading either {ggplot2} or {tidyverse} (which includes {ggplot2}) get us {ggplot2}.&lt;/p&gt;_x000D_
+&lt;p&gt;It can be confusing, but remember that {ggplot2} is the package and &lt;code&gt;ggplot()&lt;/code&gt; is the key function in that package.&lt;/p&gt;_x000D_&lt;/div&gt;</t>
         </is>
       </c>
     </row>
@@ -706,12 +746,16 @@
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>FALSE</t>
+          <t>&lt;div id="a-4" class="section level2"&gt;_x000D_
+&lt;h2&gt;A&lt;/h2&gt;_x000D_
+&lt;p&gt;FALSE&lt;/p&gt;_x000D_&lt;/div&gt;</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>TRUE</t>
+          <t>&lt;div id="b-4" class="section level2"&gt;_x000D_
+&lt;h2&gt;B&lt;/h2&gt;_x000D_
+&lt;p&gt;TRUE&lt;/p&gt;_x000D_&lt;/div&gt;</t>
         </is>
       </c>
       <c r="T6">
@@ -719,14 +763,18 @@
       </c>
       <c r="U6" t="inlineStr">
         <is>
-          <t>Correct! Only three layers have to be specified for a basic ggplot: data, aesthetics and geometries.&lt;/p&gt;
-&lt;p&gt;&lt;img src="https://drive.google.com/uc?export=view&amp;amp;id=1Qut01oSOGuBw5_7SSe-Baz0TGVsRbueJ" width="943"&gt;</t>
+          <t>&lt;div id="correct-message-4" class="section level2"&gt;_x000D_
+&lt;h2&gt;Correct message&lt;/h2&gt;_x000D_
+&lt;p&gt;Correct! Only three layers have to be specified for a basic ggplot: data, aesthetics and geometries.&lt;/p&gt;_x000D_
+&lt;p&gt;&lt;img src="https://drive.google.com/uc?export=view&amp;amp;id=1Ii1DCyFmiE5nlQeEWq1CVoudUeouuQLw" width="943"&gt;&lt;/p&gt;_x000D_&lt;/div&gt;</t>
         </is>
       </c>
       <c r="V6" t="inlineStr">
         <is>
-          <t>Only three layers have to be specified for a basic ggplot: data, aesthetics and geometries.&lt;/p&gt;
-&lt;p&gt;&lt;img src="https://drive.google.com/uc?export=view&amp;amp;id=18ungW_DEgtx8oLYr5nlFvBInCrZ3T19M" width="943"&gt;</t>
+          <t>&lt;div id="incorrect-message-4" class="section level2"&gt;_x000D_
+&lt;h2&gt;Incorrect message&lt;/h2&gt;_x000D_
+&lt;p&gt;Only three layers have to be specified for a basic ggplot: data, aesthetics and geometries.&lt;/p&gt;_x000D_
+&lt;p&gt;&lt;img src="https://drive.google.com/uc?export=view&amp;amp;id=1Z9DeB8V2ohywTBep99G199gHEnWd48in" width="943"&gt;&lt;/p&gt;_x000D_&lt;/div&gt;</t>
         </is>
       </c>
     </row>
@@ -751,17 +799,23 @@
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>Facets, data, and statistics</t>
+          <t>&lt;div id="a-5" class="section level2"&gt;_x000D_
+&lt;h2&gt;A&lt;/h2&gt;_x000D_
+&lt;p&gt;Facets, data, and statistics&lt;/p&gt;_x000D_&lt;/div&gt;</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>Coordinates, data, and themes</t>
+          <t>&lt;div id="b-5" class="section level2"&gt;_x000D_
+&lt;h2&gt;B&lt;/h2&gt;_x000D_
+&lt;p&gt;Coordinates, data, and themes&lt;/p&gt;_x000D_&lt;/div&gt;</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>Data, geometries, and aesthetics</t>
+          <t>&lt;div id="c-3" class="section level2"&gt;_x000D_
+&lt;h2&gt;C&lt;/h2&gt;_x000D_
+&lt;p&gt;Data, geometries, and aesthetics&lt;/p&gt;_x000D_&lt;/div&gt;</t>
         </is>
       </c>
       <c r="T7">
@@ -769,16 +823,19 @@
       </c>
       <c r="U7" t="inlineStr">
         <is>
-          <t>Splendid!&lt;/p&gt;
-&lt;p&gt;We need Data, Geometries, and Aesthetics for &lt;code&gt;ggplot&lt;/code&gt; to work.&lt;/p&gt;
-&lt;p&gt;&lt;img src="https://drive.google.com/uc?export=view&amp;amp;id=1A8rBVBDdT-NPjiUYh88MPAOvUoUaqaKO" width="943"&gt;</t>
+          <t>&lt;div id="correct-message-5" class="section level2"&gt;_x000D_
+&lt;h2&gt;Correct message&lt;/h2&gt;_x000D_
+&lt;p&gt;Splendid!&lt;/p&gt;_x000D_
+&lt;p&gt;We need Data, Geometries, and Aesthetics for &lt;code&gt;ggplot&lt;/code&gt; to work.&lt;/p&gt;_x000D_
+&lt;p&gt;&lt;img src="https://drive.google.com/uc?export=view&amp;amp;id=1ko6uPl2wN_kSJXJGHhBsFn_5RvTrmuL9" width="943"&gt;&lt;/p&gt;_x000D_&lt;/div&gt;</t>
         </is>
       </c>
       <c r="V7" t="inlineStr">
         <is>
-          <t>We need Data, Geometries, and Aesthetics for &lt;code&gt;ggplot&lt;/code&gt; to work.
-Go back to the lesson and see!&lt;/p&gt;
-&lt;p&gt;&lt;img src="https://drive.google.com/uc?export=view&amp;amp;id=1P7xk2sQpZ63hqN3RNWxqmPqb_ROOzgdV" width="943"&gt;</t>
+          <t>&lt;div id="incorrect-message-5" class="section level2"&gt;_x000D_
+&lt;h2&gt;Incorrect message&lt;/h2&gt;_x000D_
+&lt;p&gt;We need Data, Geometries, and Aesthetics for &lt;code&gt;ggplot&lt;/code&gt; to work. Go back to the lesson and see!&lt;/p&gt;_x000D_
+&lt;p&gt;&lt;img src="https://drive.google.com/uc?export=view&amp;amp;id=1I4uRl--b2zKe2s_TAyetLucdPiyxW5al" width="943"&gt;&lt;/p&gt;_x000D_&lt;/div&gt;</t>
         </is>
       </c>
     </row>
@@ -801,43 +858,53 @@
           <t>&lt;p&gt;All EXCEPT ONE of the code chunks shown will plot the scatter plot seen, using the &lt;code&gt;women&lt;/code&gt; dataset in R.&lt;/p&gt;
 &lt;p&gt;Which code chunk is faulty?&lt;/p&gt;
 &lt;p&gt;(Hint: &lt;code&gt;women&lt;/code&gt; is a built-in R dataset, so you can test these on your computer)&lt;/p&gt;
-&lt;p&gt;&lt;img src="https://drive.google.com/uc?export=view&amp;amp;id=1VNG7rVGGeNbDrDymSl5i4FhvpNqxCKSn" width="672"&gt;&lt;/p&gt;</t>
+&lt;p&gt;&lt;img src="https://drive.google.com/uc?export=view&amp;amp;id=15sKgpgN690kWxFntxxRi0q6lLfMnhRlL" width="672"&gt;&lt;/p&gt;</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>&lt;div id="a-6" class="section level2"&gt;&lt;pre class="r"&gt;&lt;code&gt;ggplot(data = women, 
-       mapping = aes(x = height, 
-                     y = weight)) + 
-  geom_point()&lt;/code&gt;&lt;/pre&gt;&lt;/div&gt;</t>
+          <t>&lt;div id="a-6" class="section level2"&gt;_x000D_
+&lt;h2&gt;A&lt;/h2&gt;_x000D_
+&lt;pre class="r"&gt;&lt;code&gt;ggplot(data = women, _x000D_
+       mapping = aes(x = height, _x000D_
+                     y = weight)) + _x000D_
+  geom_point()&lt;/code&gt;&lt;/pre&gt;_x000D_&lt;/div&gt;</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>&lt;div id="b-6" class="section level2"&gt;&lt;pre class="r"&gt;&lt;code&gt;ggplot(women, aes(height, weight)) + 
-  geom_point()&lt;/code&gt;&lt;/pre&gt;&lt;/div&gt;</t>
+          <t>&lt;div id="b-6" class="section level2"&gt;_x000D_
+&lt;h2&gt;B&lt;/h2&gt;_x000D_
+&lt;pre class="r"&gt;&lt;code&gt;ggplot(women, aes(height, weight)) + _x000D_
+  geom_point()&lt;/code&gt;&lt;/pre&gt;_x000D_&lt;/div&gt;</t>
         </is>
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>&lt;div id="c-4" class="section level2"&gt;&lt;pre class="r"&gt;&lt;code&gt;women %&amp;gt;% 
-  ggplot(mapping = aes(x = height, 
-                       y = weight)) + 
-  geom_point()&lt;/code&gt;&lt;/pre&gt;&lt;/div&gt;</t>
+          <t>&lt;div id="c-4" class="section level2"&gt;_x000D_
+&lt;h2&gt;C&lt;/h2&gt;_x000D_
+&lt;pre class="r"&gt;&lt;code&gt;women %&amp;gt;% _x000D_
+  ggplot(mapping = aes(x = height, _x000D_
+                       y = weight)) + _x000D_
+  geom_point()&lt;/code&gt;&lt;/pre&gt;_x000D_&lt;/div&gt;</t>
         </is>
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>&lt;div id="d-2" class="section level2"&gt;&lt;pre class="r"&gt;&lt;code&gt;women %&amp;gt;% 
-  ggplot(aes(x = height, y = weight)) + 
-  geom_point()&lt;/code&gt;&lt;/pre&gt;&lt;/div&gt;</t>
+          <t>&lt;div id="d-2" class="section level2"&gt;_x000D_
+&lt;h2&gt;D&lt;/h2&gt;_x000D_
+&lt;pre class="r"&gt;&lt;code&gt;women %&amp;gt;% _x000D_
+  ggplot(aes(x = height, y = weight)) + _x000D_
+  geom_point()&lt;/code&gt;&lt;/pre&gt;_x000D_&lt;/div&gt;</t>
         </is>
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>&lt;div id="e" class="section level2"&gt;&lt;pre class="r"&gt;&lt;code&gt;ggplot(dataset = women, 
-       aesthet = c(height, weight)) + 
-  geom_point()&lt;/code&gt;&lt;/pre&gt;&lt;/div&gt;</t>
+          <t>&lt;div id="e" class="section level2"&gt;_x000D_
+&lt;h2&gt;E&lt;/h2&gt;_x000D_
+&lt;pre class="r"&gt;&lt;code&gt;ggplot(dataset = women, _x000D_
+       aesthet = c(height, weight)) + _x000D_
+  geom_point()&lt;/code&gt;&lt;/pre&gt;_x000D_&lt;/div&gt;</t>
         </is>
       </c>
       <c r="T8">
@@ -845,31 +912,34 @@
       </c>
       <c r="U8" t="inlineStr">
         <is>
-          <t>Great catch!&lt;/p&gt;
-&lt;p&gt;&lt;code&gt;dataset&lt;/code&gt; and &lt;code&gt;aesthet&lt;/code&gt; are incorrect arguments of &lt;code&gt;ggplot()&lt;/code&gt;.&lt;/p&gt;
-&lt;p&gt;As you can see, there are many ways to write correct ggplot code.&lt;/p&gt;
-&lt;p&gt;In this example, the most explicit code would be:&lt;/p&gt;
-&lt;pre class="r"&gt;&lt;code&gt;ggplot(data = women, 
-       mapping = aes(x = height, y = weight)) + 
-  geom_point()&lt;/code&gt;&lt;/pre&gt;
-&lt;p&gt;But we can skip the argument names as long as we provide the data and the aesthetic mappings as the first and second arguments (because R matches arguments by position):&lt;/p&gt;
-&lt;pre class="r"&gt;&lt;code&gt;ggplot(women, aes(x = height, y = weight)) + 
-  geom_point()&lt;/code&gt;&lt;/pre&gt;
-&lt;p&gt;Similarly, &lt;code&gt;x&lt;/code&gt; and &lt;code&gt;y&lt;/code&gt; are the first and second arguments in the &lt;code&gt;aes()&lt;/code&gt; function, so if we provide the argument values in the right order, we can skip &lt;code&gt;x =&lt;/code&gt; and &lt;code&gt;y =&lt;/code&gt; in the code</t>
+          <t>&lt;div id="correct-message-6" class="section level2"&gt;_x000D_
+&lt;h2&gt;Correct message&lt;/h2&gt;_x000D_
+&lt;p&gt;Great catch!&lt;/p&gt;_x000D_
+&lt;p&gt;&lt;code&gt;dataset&lt;/code&gt; and &lt;code&gt;aesthet&lt;/code&gt; are incorrect arguments of &lt;code&gt;ggplot()&lt;/code&gt;.&lt;/p&gt;_x000D_
+&lt;p&gt;As you can see, there are many ways to write correct ggplot code.&lt;/p&gt;_x000D_
+&lt;p&gt;In this example, the most explicit code would be:&lt;/p&gt;_x000D_
+&lt;pre class="r"&gt;&lt;code&gt;ggplot(data = women, _x000D_
+       mapping = aes(x = height, y = weight)) + _x000D_
+  geom_point()&lt;/code&gt;&lt;/pre&gt;_x000D_
+&lt;p&gt;But we can skip the argument names as long as we provide the data and the aesthetic mappings as the first and second arguments (because R matches arguments by position):&lt;/p&gt;_x000D_
+&lt;pre class="r"&gt;&lt;code&gt;ggplot(women, aes(x = height, y = weight)) + _x000D_
+  geom_point()&lt;/code&gt;&lt;/pre&gt;_x000D_
+&lt;p&gt;Similarly, &lt;code&gt;x&lt;/code&gt; and &lt;code&gt;y&lt;/code&gt; are the first and second arguments in the &lt;code&gt;aes()&lt;/code&gt; function, so if we provide the argument values in the right order, we can skip &lt;code&gt;x =&lt;/code&gt; and &lt;code&gt;y =&lt;/code&gt; in the code&lt;/p&gt;_x000D_&lt;/div&gt;</t>
         </is>
       </c>
       <c r="V8" t="inlineStr">
         <is>
-          <t>&lt;code&gt;dataset&lt;/code&gt; and &lt;code&gt;aesthet&lt;/code&gt; are incorrect arguments of &lt;code&gt;ggplot()&lt;/code&gt;.&lt;/p&gt;
-&lt;p&gt;As you can see, there are many ways to write correct ggplot code.
-In this example, the most explicit code would be:&lt;/p&gt;
-&lt;pre class="r"&gt;&lt;code&gt;ggplot(data = women, 
-       mapping = aes(x = height, y = weight)) + 
-  geom_point()&lt;/code&gt;&lt;/pre&gt;
-&lt;p&gt;But we can skip the argument names as long as we provide the data and the aesthetic mappings as the first and second arguments (because R matches arguments by position):&lt;/p&gt;
-&lt;pre class="r"&gt;&lt;code&gt;ggplot(women, aes(x = height, y = weight)) + 
-  geom_point()&lt;/code&gt;&lt;/pre&gt;
-&lt;p&gt;Similarly, &lt;code&gt;x&lt;/code&gt; and &lt;code&gt;y&lt;/code&gt; are the first and second arguments in the &lt;code&gt;aes()&lt;/code&gt; function, so if we provide the argument values in the right order, we can skip &lt;code&gt;x =&lt;/code&gt; and &lt;code&gt;y =&lt;/code&gt; in the code</t>
+          <t>&lt;div id="incorrect-message-6" class="section level2"&gt;_x000D_
+&lt;h2&gt;Incorrect message&lt;/h2&gt;_x000D_
+&lt;p&gt;&lt;code&gt;dataset&lt;/code&gt; and &lt;code&gt;aesthet&lt;/code&gt; are incorrect arguments of &lt;code&gt;ggplot()&lt;/code&gt;.&lt;/p&gt;_x000D_
+&lt;p&gt;As you can see, there are many ways to write correct ggplot code. In this example, the most explicit code would be:&lt;/p&gt;_x000D_
+&lt;pre class="r"&gt;&lt;code&gt;ggplot(data = women, _x000D_
+       mapping = aes(x = height, y = weight)) + _x000D_
+  geom_point()&lt;/code&gt;&lt;/pre&gt;_x000D_
+&lt;p&gt;But we can skip the argument names as long as we provide the data and the aesthetic mappings as the first and second arguments (because R matches arguments by position):&lt;/p&gt;_x000D_
+&lt;pre class="r"&gt;&lt;code&gt;ggplot(women, aes(x = height, y = weight)) + _x000D_
+  geom_point()&lt;/code&gt;&lt;/pre&gt;_x000D_
+&lt;p&gt;Similarly, &lt;code&gt;x&lt;/code&gt; and &lt;code&gt;y&lt;/code&gt; are the first and second arguments in the &lt;code&gt;aes()&lt;/code&gt; function, so if we provide the argument values in the right order, we can skip &lt;code&gt;x =&lt;/code&gt; and &lt;code&gt;y =&lt;/code&gt; in the code&lt;/p&gt;_x000D_&lt;/div&gt;</t>
         </is>
       </c>
     </row>
@@ -890,29 +960,34 @@
       <c r="F9" t="inlineStr">
         <is>
           <t>&lt;p&gt;The scatterplot below uses the &lt;code&gt;storms&lt;/code&gt; dataset from {dplyr} to visualize the positions and movements of hurricanes in the Unites States in the year 2005.&lt;/p&gt;
-&lt;pre class="r"&gt;&lt;code&gt;hurricanes &amp;lt;- storms  %&amp;gt;% filter(status == "hurricane", year == 2005)
-ggplot(data = hurricanes, 
-       mapping = aes(x = long, y = lat, color = name)) + 
+&lt;pre class="r"&gt;&lt;code&gt;hurricanes &amp;lt;- storms  %&amp;gt;% filter(status == "hurricane", year == 2005)_x000D_
+_x000D_
+ggplot(data = hurricanes, _x000D_
+       mapping = aes(x = long, y = lat, color = name)) + _x000D_
   geom_point()&lt;/code&gt;&lt;/pre&gt;
-&lt;p&gt;&lt;img src="https://drive.google.com/uc?export=view&amp;amp;id=1Pi1uErVKBlNA3eno0K_IFNL27O3GR9_O" width="672"&gt;&lt;/p&gt;
+&lt;p&gt;&lt;img src="https://drive.google.com/uc?export=view&amp;amp;id=1nYrsAZHvlbvYJYmS9Bua_z5hI9FEAc5u" width="672"&gt;&lt;/p&gt;
 &lt;p&gt;Which of the options below correctly describes the aesthetic mappings of this plot?&lt;/p&gt;</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>&lt;div id="a-7" class="section level2"&gt;&lt;ul&gt;
-&lt;li&gt;The latitude variable is mapped to the x aesthetic&lt;/li&gt;
-&lt;li&gt;The longitude variable is mapped to y aesthetic&lt;/li&gt;
-&lt;li&gt;The name variable is mapped to the color aesthetic&lt;/li&gt;
+          <t>&lt;div id="a-7" class="section level2"&gt;_x000D_
+&lt;h2&gt;A&lt;/h2&gt;_x000D_
+&lt;ul&gt;
+&lt;li&gt;The latitude variable is mapped to the x aesthetic&lt;/li&gt;_x000D_
+&lt;li&gt;The longitude variable is mapped to y aesthetic&lt;/li&gt;_x000D_
+&lt;li&gt;The name variable is mapped to the color aesthetic&lt;/li&gt;_x000D_
 &lt;/ul&gt;&lt;/div&gt;</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>&lt;div id="b-7" class="section level2"&gt;&lt;ul&gt;
-&lt;li&gt;The latitude aesthetic is mapped to the x axis&lt;/li&gt;
-&lt;li&gt;The longitude aesthetic is mapped to y axis&lt;/li&gt;
-&lt;li&gt;The name aesthetic is mapped to the point color&lt;/li&gt;
+          <t>&lt;div id="b-7" class="section level2"&gt;_x000D_
+&lt;h2&gt;B&lt;/h2&gt;_x000D_
+&lt;ul&gt;
+&lt;li&gt;The latitude aesthetic is mapped to the x axis&lt;/li&gt;_x000D_
+&lt;li&gt;The longitude aesthetic is mapped to y axis&lt;/li&gt;_x000D_
+&lt;li&gt;The name aesthetic is mapped to the point color&lt;/li&gt;_x000D_
 &lt;/ul&gt;&lt;/div&gt;</t>
         </is>
       </c>
@@ -921,15 +996,19 @@
       </c>
       <c r="U9" t="inlineStr">
         <is>
-          <t>Looks like you got it!&lt;/p&gt;
-&lt;p&gt;The aesthetics used in this plot are x, y and color. Each of these aesthetics is mapped to variable from the data.&lt;/p&gt;
-&lt;p&gt;Remember that the word “map” used here does not refer to a geographic map! When we say something like “the name variable is mapped to the color aesthetic” we mean “the name variable is &lt;em&gt;represented by&lt;/em&gt; or &lt;em&gt;linked to&lt;/em&gt; the color aesthetic”.</t>
+          <t>&lt;div id="correct-message-7" class="section level2"&gt;_x000D_
+&lt;h2&gt;Correct message&lt;/h2&gt;_x000D_
+&lt;p&gt;Looks like you got it!&lt;/p&gt;_x000D_
+&lt;p&gt;The aesthetics used in this plot are x, y and color. Each of these aesthetics is mapped to variable from the data.&lt;/p&gt;_x000D_
+&lt;p&gt;Remember that the word “map” used here does not refer to a geographic map! When we say something like “the name variable is mapped to the color aesthetic” we mean “the name variable is &lt;em&gt;represented by&lt;/em&gt; or &lt;em&gt;linked to&lt;/em&gt; the color aesthetic”.&lt;/p&gt;_x000D_&lt;/div&gt;</t>
         </is>
       </c>
       <c r="V9" t="inlineStr">
         <is>
-          <t>The aesthetics used in this plot are x, y and color. Each of these aesthetics is mapped to variable from the data.&lt;/p&gt;
-&lt;p&gt;Remember that the word “map” used here does not refer to a geographic map! When we say something like “the name variable is mapped to the color aesthetic” we mean “the name variable is &lt;em&gt;represented by&lt;/em&gt; or &lt;em&gt;linked to&lt;/em&gt; the color aesthetic”.</t>
+          <t>&lt;div id="incorrect-message-7" class="section level2"&gt;_x000D_
+&lt;h2&gt;Incorrect message&lt;/h2&gt;_x000D_
+&lt;p&gt;The aesthetics used in this plot are x, y and color. Each of these aesthetics is mapped to variable from the data.&lt;/p&gt;_x000D_
+&lt;p&gt;Remember that the word “map” used here does not refer to a geographic map! When we say something like “the name variable is mapped to the color aesthetic” we mean “the name variable is &lt;em&gt;represented by&lt;/em&gt; or &lt;em&gt;linked to&lt;/em&gt; the color aesthetic”.&lt;/p&gt;_x000D_&lt;/div&gt;</t>
         </is>
       </c>
     </row>
@@ -954,22 +1033,30 @@
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>the &lt;code&gt;aes&lt;/code&gt; layer</t>
+          <t>&lt;div id="a-8" class="section level2"&gt;_x000D_
+&lt;h2&gt;A&lt;/h2&gt;_x000D_
+&lt;p&gt;the &lt;code&gt;aes&lt;/code&gt; layer&lt;/p&gt;_x000D_&lt;/div&gt;</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>the &lt;code&gt;geom&lt;/code&gt; layer</t>
+          <t>&lt;div id="b-8" class="section level2"&gt;_x000D_
+&lt;h2&gt;B&lt;/h2&gt;_x000D_
+&lt;p&gt;the &lt;code&gt;geom&lt;/code&gt; layer&lt;/p&gt;_x000D_&lt;/div&gt;</t>
         </is>
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>the &lt;code&gt;statistics&lt;/code&gt; layer</t>
+          <t>&lt;div id="c-5" class="section level2"&gt;_x000D_
+&lt;h2&gt;C&lt;/h2&gt;_x000D_
+&lt;p&gt;the &lt;code&gt;statistics&lt;/code&gt; layer&lt;/p&gt;_x000D_&lt;/div&gt;</t>
         </is>
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>the &lt;code&gt;data&lt;/code&gt; layer</t>
+          <t>&lt;div id="d-3" class="section level2"&gt;_x000D_
+&lt;h2&gt;D&lt;/h2&gt;_x000D_
+&lt;p&gt;the &lt;code&gt;data&lt;/code&gt; layer&lt;/p&gt;_x000D_&lt;/div&gt;</t>
         </is>
       </c>
       <c r="T10">
@@ -977,24 +1064,27 @@
       </c>
       <c r="U10" t="inlineStr">
         <is>
-          <t>Exactly right!&lt;/p&gt;
-&lt;p&gt;It’s defined with the &lt;code&gt;aes&lt;/code&gt;thetic layer.&lt;/p&gt;
-&lt;p&gt;For example:&lt;/p&gt;
-&lt;pre class="r"&gt;&lt;code&gt;ggplot(iris, 
-       aes(x = Petal.Length, y = Petal.Width, color = Species)) + ## aesthetic layer
-  geom_point()&lt;/code&gt;&lt;/pre&gt;
-&lt;p&gt;&lt;img src="https://drive.google.com/uc?export=view&amp;amp;id=1Gtc685B6Wmnywyi0_QMiyGRRaV8_Kzhc" width="672"&gt;</t>
+          <t>&lt;div id="correct-message-8" class="section level2"&gt;_x000D_
+&lt;h2&gt;Correct message&lt;/h2&gt;_x000D_
+&lt;p&gt;Exactly right!&lt;/p&gt;_x000D_
+&lt;p&gt;It’s defined with the &lt;code&gt;aes&lt;/code&gt;thetic layer.&lt;/p&gt;_x000D_
+&lt;p&gt;For example:&lt;/p&gt;_x000D_
+&lt;pre class="r"&gt;&lt;code&gt;ggplot(iris, _x000D_
+       aes(x = Petal.Length, y = Petal.Width, color = Species)) + ## aesthetic layer_x000D_
+  geom_point()&lt;/code&gt;&lt;/pre&gt;_x000D_
+&lt;p&gt;&lt;img src="https://drive.google.com/uc?export=view&amp;amp;id=1uShts-pcM72ZfqY6X7ZdP_rPYU7BZnP3" width="672"&gt;&lt;/p&gt;_x000D_&lt;/div&gt;</t>
         </is>
       </c>
       <c r="V10" t="inlineStr">
         <is>
-          <t>Sorry, that’s not it!&lt;/p&gt;
-&lt;p&gt;It’s defined with the &lt;code&gt;aes&lt;/code&gt;thetic layer.
-For example:&lt;/p&gt;
-&lt;pre class="r"&gt;&lt;code&gt;ggplot(iris, 
-       aes(x = Petal.Length, y = Petal.Width, color = Species)) + ## aesthetic layer
-  geom_point()&lt;/code&gt;&lt;/pre&gt;
-&lt;p&gt;&lt;img src="https://drive.google.com/uc?export=view&amp;amp;id=1SUwCkXVsJMT6TnY9ekkr_O_mL7tFp0kE" width="672"&gt;</t>
+          <t>&lt;div id="incorrect-message-8" class="section level2"&gt;_x000D_
+&lt;h2&gt;Incorrect message&lt;/h2&gt;_x000D_
+&lt;p&gt;Sorry, that’s not it!&lt;/p&gt;_x000D_
+&lt;p&gt;It’s defined with the &lt;code&gt;aes&lt;/code&gt;thetic layer. For example:&lt;/p&gt;_x000D_
+&lt;pre class="r"&gt;&lt;code&gt;ggplot(iris, _x000D_
+       aes(x = Petal.Length, y = Petal.Width, color = Species)) + ## aesthetic layer_x000D_
+  geom_point()&lt;/code&gt;&lt;/pre&gt;_x000D_
+&lt;p&gt;&lt;img src="https://drive.google.com/uc?export=view&amp;amp;id=12acPgjFaYpqFWNYTdGJcq8Rm7dJCzPEU" width="672"&gt;&lt;/p&gt;_x000D_&lt;/div&gt;</t>
         </is>
       </c>
     </row>
@@ -1019,17 +1109,23 @@
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>&lt;div id="a-9" class="section level2"&gt;&lt;pre class="r"&gt;&lt;code&gt;ggplot(data=dengue)&lt;/code&gt;&lt;/pre&gt;&lt;/div&gt;</t>
+          <t>&lt;div id="a-9" class="section level2"&gt;_x000D_
+&lt;h2&gt;A&lt;/h2&gt;_x000D_
+&lt;pre class="r"&gt;&lt;code&gt;ggplot(data=dengue)&lt;/code&gt;&lt;/pre&gt;_x000D_&lt;/div&gt;</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>&lt;div id="b-9" class="section level2"&gt;&lt;pre class="r"&gt;&lt;code&gt;ggplot() + data(dengue)&lt;/code&gt;&lt;/pre&gt;&lt;/div&gt;</t>
+          <t>&lt;div id="b-9" class="section level2"&gt;_x000D_
+&lt;h2&gt;B&lt;/h2&gt;_x000D_
+&lt;pre class="r"&gt;&lt;code&gt;ggplot() + data(dengue)&lt;/code&gt;&lt;/pre&gt;_x000D_&lt;/div&gt;</t>
         </is>
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>&lt;div id="c-6" class="section level2"&gt;&lt;pre class="r"&gt;&lt;code&gt;ggplot.data(dengue)&lt;/code&gt;&lt;/pre&gt;&lt;/div&gt;</t>
+          <t>&lt;div id="c-6" class="section level2"&gt;_x000D_
+&lt;h2&gt;C&lt;/h2&gt;_x000D_
+&lt;pre class="r"&gt;&lt;code&gt;ggplot.data(dengue)&lt;/code&gt;&lt;/pre&gt;_x000D_&lt;/div&gt;</t>
         </is>
       </c>
       <c r="T11">
@@ -1037,13 +1133,17 @@
       </c>
       <c r="U11" t="inlineStr">
         <is>
-          <t>That’s the one!&lt;/p&gt;
-&lt;p&gt;Remember that you can type in &lt;code&gt;?ggplot&lt;/code&gt; into your R console to see how to properly define the arguments for this function.</t>
+          <t>&lt;div id="correct-message-9" class="section level2"&gt;_x000D_
+&lt;h2&gt;Correct message&lt;/h2&gt;_x000D_
+&lt;p&gt;That’s the one!&lt;/p&gt;_x000D_
+&lt;p&gt;Remember that you can type in &lt;code&gt;?ggplot&lt;/code&gt; into your R console to see how to properly define the arguments for this function.&lt;/p&gt;_x000D_&lt;/div&gt;</t>
         </is>
       </c>
       <c r="V11" t="inlineStr">
         <is>
-          <t>Remember that you can type in &lt;code&gt;?ggplot&lt;/code&gt; into your R console to see how to properly define the arguments for this function.</t>
+          <t>&lt;div id="incorrect-message-9" class="section level2"&gt;_x000D_
+&lt;h2&gt;Incorrect message&lt;/h2&gt;_x000D_
+&lt;p&gt;Remember that you can type in &lt;code&gt;?ggplot&lt;/code&gt; into your R console to see how to properly define the arguments for this function.&lt;/p&gt;_x000D_&lt;/div&gt;</t>
         </is>
       </c>
     </row>
@@ -1064,25 +1164,31 @@
       <c r="F12" t="inlineStr">
         <is>
           <t>&lt;p&gt;The code below tries to use the &lt;code&gt;swiss&lt;/code&gt; dataset (a built-in R dataset) to create a scatter plot of &lt;code&gt;Infant.Mortality&lt;/code&gt; against &lt;code&gt;Fertility&lt;/code&gt;, but generates a blank plot due to an error/oversight.&lt;/p&gt;
-&lt;pre class="r"&gt;&lt;code&gt;ggplot(data = swiss, 
-       mapping = aes(x = Fertility, 
+&lt;pre class="r"&gt;&lt;code&gt;ggplot(data = swiss, _x000D_
+       mapping = aes(x = Fertility, _x000D_
                      y = Infant.Mortality))&lt;/code&gt;&lt;/pre&gt;
 &lt;p&gt;What is the problem with the code above?&lt;/p&gt;</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>It is missing a data layer</t>
+          <t>&lt;div id="a-10" class="section level2"&gt;_x000D_
+&lt;h2&gt;A&lt;/h2&gt;_x000D_
+&lt;p&gt;It is missing a data layer&lt;/p&gt;_x000D_&lt;/div&gt;</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>It is missing an aesthetic mapping</t>
+          <t>&lt;div id="b-10" class="section level2"&gt;_x000D_
+&lt;h2&gt;B&lt;/h2&gt;_x000D_
+&lt;p&gt;It is missing an aesthetic mapping&lt;/p&gt;_x000D_&lt;/div&gt;</t>
         </is>
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>It is missing a geometric function</t>
+          <t>&lt;div id="c-7" class="section level2"&gt;_x000D_
+&lt;h2&gt;C&lt;/h2&gt;_x000D_
+&lt;p&gt;It is missing a geometric function&lt;/p&gt;_x000D_&lt;/div&gt;</t>
         </is>
       </c>
       <c r="T12">
@@ -1090,22 +1196,26 @@
       </c>
       <c r="U12" t="inlineStr">
         <is>
-          <t>Nice work! The data layer and aesthetic mappings are properly specified, but there is no &lt;code&gt;geom_*&lt;/code&gt; function. In this case, &lt;code&gt;geom_point()&lt;/code&gt; is needed:&lt;/p&gt;
-&lt;pre class="r"&gt;&lt;code&gt;ggplot(data = swiss, 
-       mapping = aes(x = Fertility, 
-                     y = Infant.Mortality)) + 
-  geom_point()&lt;/code&gt;&lt;/pre&gt;
-&lt;p&gt;&lt;img src="https://drive.google.com/uc?export=view&amp;amp;id=1O1RwYEFvc5L8WHf6lFfO4M-QROlYN6RL" width="672"&gt;</t>
+          <t>&lt;div id="correct-message-10" class="section level2"&gt;_x000D_
+&lt;h2&gt;Correct message&lt;/h2&gt;_x000D_
+&lt;p&gt;Nice work! The data layer and aesthetic mappings are properly specified, but there is no &lt;code&gt;geom_*&lt;/code&gt; function. In this case, &lt;code&gt;geom_point()&lt;/code&gt; is needed:&lt;/p&gt;_x000D_
+&lt;pre class="r"&gt;&lt;code&gt;ggplot(data = swiss, _x000D_
+       mapping = aes(x = Fertility, _x000D_
+                     y = Infant.Mortality)) + _x000D_
+  geom_point()&lt;/code&gt;&lt;/pre&gt;_x000D_
+&lt;p&gt;&lt;img src="https://drive.google.com/uc?export=view&amp;amp;id=1s7yfkvnhwoP1wWnNjy4knTbgrnNHV50-" width="672"&gt;&lt;/p&gt;_x000D_&lt;/div&gt;</t>
         </is>
       </c>
       <c r="V12" t="inlineStr">
         <is>
-          <t>The data layer and aesthetic mappings are properly specified, but there is no &lt;code&gt;geom_*&lt;/code&gt; function. In this case, &lt;code&gt;geom_point()&lt;/code&gt; is needed:&lt;/p&gt;
-&lt;pre class="r"&gt;&lt;code&gt;ggplot(data = swiss, 
-       mapping = aes(x = Fertility, 
-                     y = Infant.Mortality)) + 
-  geom_point()&lt;/code&gt;&lt;/pre&gt;
-&lt;p&gt;&lt;img src="https://drive.google.com/uc?export=view&amp;amp;id=1FaGdPV-tMD-xAiXO1mSbB9EyzF6Q8zbk" width="672"&gt;</t>
+          <t>&lt;div id="incorrect-message-10" class="section level2"&gt;_x000D_
+&lt;h2&gt;Incorrect message&lt;/h2&gt;_x000D_
+&lt;p&gt;The data layer and aesthetic mappings are properly specified, but there is no &lt;code&gt;geom_*&lt;/code&gt; function. In this case, &lt;code&gt;geom_point()&lt;/code&gt; is needed:&lt;/p&gt;_x000D_
+&lt;pre class="r"&gt;&lt;code&gt;ggplot(data = swiss, _x000D_
+       mapping = aes(x = Fertility, _x000D_
+                     y = Infant.Mortality)) + _x000D_
+  geom_point()&lt;/code&gt;&lt;/pre&gt;_x000D_
+&lt;p&gt;&lt;img src="https://drive.google.com/uc?export=view&amp;amp;id=1II2hPj5YHRAbvNRT9yXEzaBWkP6CSJK4" width="672"&gt;&lt;/p&gt;_x000D_&lt;/div&gt;</t>
         </is>
       </c>
     </row>
@@ -1127,24 +1237,30 @@
         <is>
           <t>&lt;p&gt;The code below attempts to create a scatterplot of weight against height using the &lt;code&gt;women&lt;/code&gt; dataset (a built-in R dataset).&lt;/p&gt;
 &lt;p&gt;The code is faulty however, and generates no plot.&lt;/p&gt;
-&lt;pre class="r"&gt;&lt;code&gt;ggplot(women, aes(x = height, y = weight)) %&amp;gt;% 
+&lt;pre class="r"&gt;&lt;code&gt;ggplot(women, aes(x = height, y = weight)) %&amp;gt;% _x000D_
   geom_point()&lt;/code&gt;&lt;/pre&gt;
 &lt;p&gt;Which of the options below accurately describes the issue with the code?&lt;/p&gt;</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>The code is missing the x and y aesthetic mappings.</t>
+          <t>&lt;div id="a-11" class="section level2"&gt;_x000D_
+&lt;h2&gt;A&lt;/h2&gt;_x000D_
+&lt;p&gt;The code is missing the x and y aesthetic mappings.&lt;/p&gt;_x000D_&lt;/div&gt;</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>The code uses &lt;code&gt;%&amp;gt;%&lt;/code&gt; instead of &lt;code&gt;+&lt;/code&gt; to link the layers of the ggplot.</t>
+          <t>&lt;div id="b-11" class="section level2"&gt;_x000D_
+&lt;h2&gt;B&lt;/h2&gt;_x000D_
+&lt;p&gt;The code uses &lt;code&gt;%&amp;gt;%&lt;/code&gt; instead of &lt;code&gt;+&lt;/code&gt; to link the layers of the ggplot.&lt;/p&gt;_x000D_&lt;/div&gt;</t>
         </is>
       </c>
       <c r="I13" t="inlineStr">
         <is>
-          <t>The code is missing the &lt;code&gt;data&lt;/code&gt; argument to ggplot.</t>
+          <t>&lt;div id="c-8" class="section level2"&gt;_x000D_
+&lt;h2&gt;C&lt;/h2&gt;_x000D_
+&lt;p&gt;The code is missing the &lt;code&gt;data&lt;/code&gt; argument to ggplot.&lt;/p&gt;_x000D_&lt;/div&gt;</t>
         </is>
       </c>
       <c r="T13">
@@ -1152,25 +1268,29 @@
       </c>
       <c r="U13" t="inlineStr">
         <is>
-          <t>Great work!&lt;/p&gt;
-&lt;p&gt;Indeed the code uses uses &lt;code&gt;%&amp;gt;%&lt;/code&gt; instead of &lt;code&gt;+&lt;/code&gt;. This is a common error when plotting with ggplot. Luckily, ggplot2 now gives you a helpful warning when you make this mistake.&lt;/p&gt;
-&lt;p&gt;As for the other two options, remember that in R, function arguments can be matched by position, without explicitly naming the arguments.&lt;/p&gt;
-&lt;p&gt;So, the abbreviated&lt;/p&gt;
-&lt;pre class="r"&gt;&lt;code&gt;ggplot(women, aes(x = height, y = weight))&lt;/code&gt;&lt;/pre&gt;
-&lt;p&gt;and the longer&lt;/p&gt;
-&lt;pre class="r"&gt;&lt;code&gt;ggplot(data = women, mapping = aes(x = height, y = weight))&lt;/code&gt;&lt;/pre&gt;
-&lt;p&gt;are functionally equivalent.</t>
+          <t>&lt;div id="correct-message-11" class="section level2"&gt;_x000D_
+&lt;h2&gt;Correct message&lt;/h2&gt;_x000D_
+&lt;p&gt;Great work!&lt;/p&gt;_x000D_
+&lt;p&gt;Indeed the code uses uses &lt;code&gt;%&amp;gt;%&lt;/code&gt; instead of &lt;code&gt;+&lt;/code&gt;. This is a common error when plotting with ggplot. Luckily, ggplot2 now gives you a helpful warning when you make this mistake.&lt;/p&gt;_x000D_
+&lt;p&gt;As for the other two options, remember that in R, function arguments can be matched by position, without explicitly naming the arguments.&lt;/p&gt;_x000D_
+&lt;p&gt;So, the abbreviated&lt;/p&gt;_x000D_
+&lt;pre class="r"&gt;&lt;code&gt;ggplot(women, aes(x = height, y = weight))&lt;/code&gt;&lt;/pre&gt;_x000D_
+&lt;p&gt;and the longer&lt;/p&gt;_x000D_
+&lt;pre class="r"&gt;&lt;code&gt;ggplot(data = women, mapping = aes(x = height, y = weight))&lt;/code&gt;&lt;/pre&gt;_x000D_
+&lt;p&gt;are functionally equivalent.&lt;/p&gt;_x000D_&lt;/div&gt;</t>
         </is>
       </c>
       <c r="V13" t="inlineStr">
         <is>
-          <t>The code uses uses &lt;code&gt;%&amp;gt;%&lt;/code&gt; instead of &lt;code&gt;+&lt;/code&gt;. This is a common error when plotting with ggplot. Luckily, ggplot2 now gives you a helpful warning when you make this mistake.&lt;/p&gt;
-&lt;p&gt;As for the other two options, remember that in R, function arguments can be matched by position, without explicitly naming the arguments.&lt;/p&gt;
-&lt;p&gt;So, the abbreviated&lt;/p&gt;
-&lt;pre class="r"&gt;&lt;code&gt;ggplot(women, aes(x = height, y = weight))&lt;/code&gt;&lt;/pre&gt;
-&lt;p&gt;and the longer&lt;/p&gt;
-&lt;pre class="r"&gt;&lt;code&gt;ggplot(data = women, mapping = aes(x = height, y = weight))&lt;/code&gt;&lt;/pre&gt;
-&lt;p&gt;are functionally equivalent.</t>
+          <t>&lt;div id="incorrect-message-11" class="section level2"&gt;_x000D_
+&lt;h2&gt;Incorrect message&lt;/h2&gt;_x000D_
+&lt;p&gt;The code uses uses &lt;code&gt;%&amp;gt;%&lt;/code&gt; instead of &lt;code&gt;+&lt;/code&gt;. This is a common error when plotting with ggplot. Luckily, ggplot2 now gives you a helpful warning when you make this mistake.&lt;/p&gt;_x000D_
+&lt;p&gt;As for the other two options, remember that in R, function arguments can be matched by position, without explicitly naming the arguments.&lt;/p&gt;_x000D_
+&lt;p&gt;So, the abbreviated&lt;/p&gt;_x000D_
+&lt;pre class="r"&gt;&lt;code&gt;ggplot(women, aes(x = height, y = weight))&lt;/code&gt;&lt;/pre&gt;_x000D_
+&lt;p&gt;and the longer&lt;/p&gt;_x000D_
+&lt;pre class="r"&gt;&lt;code&gt;ggplot(data = women, mapping = aes(x = height, y = weight))&lt;/code&gt;&lt;/pre&gt;_x000D_
+&lt;p&gt;are functionally equivalent.&lt;/p&gt;_x000D_&lt;/div&gt;</t>
         </is>
       </c>
     </row>
@@ -1191,24 +1311,30 @@
       <c r="F14" t="inlineStr">
         <is>
           <t>&lt;p&gt;You try to plot a graph with the following code:&lt;/p&gt;
-&lt;pre class="r"&gt;&lt;code&gt;ggplot(mapping = aes(x = height, y = weight)) +
+&lt;pre class="r"&gt;&lt;code&gt;ggplot(mapping = aes(x = height, y = weight)) +_x000D_
   geom_point()&lt;/code&gt;&lt;/pre&gt;
 &lt;p&gt;but R returns an error message. What is the problem with this code?&lt;/p&gt;</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>No color has been defined for the plot, so all the data points are transparent.</t>
+          <t>&lt;div id="a-12" class="section level2"&gt;_x000D_
+&lt;h2&gt;A&lt;/h2&gt;_x000D_
+&lt;p&gt;No color has been defined for the plot, so all the data points are transparent.&lt;/p&gt;_x000D_&lt;/div&gt;</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>No geometric layer has been defined yet.</t>
+          <t>&lt;div id="b-12" class="section level2"&gt;_x000D_
+&lt;h2&gt;B&lt;/h2&gt;_x000D_
+&lt;p&gt;No geometric layer has been defined yet.&lt;/p&gt;_x000D_&lt;/div&gt;</t>
         </is>
       </c>
       <c r="I14" t="inlineStr">
         <is>
-          <t>No dataset has been provided yet.</t>
+          <t>&lt;div id="c-9" class="section level2"&gt;_x000D_
+&lt;h2&gt;C&lt;/h2&gt;_x000D_
+&lt;p&gt;No dataset has been provided yet.&lt;/p&gt;_x000D_&lt;/div&gt;</t>
         </is>
       </c>
       <c r="T14">
@@ -1216,22 +1342,26 @@
       </c>
       <c r="U14" t="inlineStr">
         <is>
-          <t>&lt;strong&gt;G&lt;/strong&gt;ood &lt;strong&gt;g&lt;/strong&gt;ame! The data for ggplot to use has not been specified.&lt;/p&gt;
-&lt;p&gt;Here is the correct call, and the resulting output:&lt;/p&gt;
-&lt;pre class="r"&gt;&lt;code&gt;ggplot(data = women, 
-       mapping = aes(x = height, y = weight)) + 
-  geom_point()&lt;/code&gt;&lt;/pre&gt;
-&lt;p&gt;&lt;img src="https://drive.google.com/uc?export=view&amp;amp;id=1iOsgTwC7jlWQMj1WxoGxmpBsYEPkqi4p" width="672"&gt;</t>
+          <t>&lt;div id="correct-message-12" class="section level2"&gt;_x000D_
+&lt;h2&gt;Correct message&lt;/h2&gt;_x000D_
+&lt;p&gt;&lt;strong&gt;G&lt;/strong&gt;ood &lt;strong&gt;g&lt;/strong&gt;ame! The data for ggplot to use has not been specified.&lt;/p&gt;_x000D_
+&lt;p&gt;Here is the correct call, and the resulting output:&lt;/p&gt;_x000D_
+&lt;pre class="r"&gt;&lt;code&gt;ggplot(data = women, _x000D_
+       mapping = aes(x = height, y = weight)) + _x000D_
+  geom_point()&lt;/code&gt;&lt;/pre&gt;_x000D_
+&lt;p&gt;&lt;img src="https://drive.google.com/uc?export=view&amp;amp;id=1Ob3N1MX65EFbVRHNb9Bea9jgr2OyPQE3" width="672"&gt;&lt;/p&gt;_x000D_&lt;/div&gt;</t>
         </is>
       </c>
       <c r="V14" t="inlineStr">
         <is>
-          <t>The data for ggplot to use has not been specified.&lt;/p&gt;
-&lt;p&gt;Here is the correct call, and the resulting output:&lt;/p&gt;
-&lt;pre class="r"&gt;&lt;code&gt;ggplot(data = women, 
-       mapping = aes(x = height, y = weight)) + 
-  geom_point()&lt;/code&gt;&lt;/pre&gt;
-&lt;p&gt;&lt;img src="https://drive.google.com/uc?export=view&amp;amp;id=1qZg0lEiLkH3hZFCfONx29FSWmHY6AXWB" width="672"&gt;</t>
+          <t>&lt;div id="incorrect-message-12" class="section level2"&gt;_x000D_
+&lt;h2&gt;Incorrect message&lt;/h2&gt;_x000D_
+&lt;p&gt;The data for ggplot to use has not been specified.&lt;/p&gt;_x000D_
+&lt;p&gt;Here is the correct call, and the resulting output:&lt;/p&gt;_x000D_
+&lt;pre class="r"&gt;&lt;code&gt;ggplot(data = women, _x000D_
+       mapping = aes(x = height, y = weight)) + _x000D_
+  geom_point()&lt;/code&gt;&lt;/pre&gt;_x000D_
+&lt;p&gt;&lt;img src="https://drive.google.com/uc?export=view&amp;amp;id=1IjRgcEAGFP0FyquhsNfhHrJCa7vbcMXW" width="672"&gt;&lt;/p&gt;_x000D_&lt;/div&gt;</t>
         </is>
       </c>
     </row>
@@ -1252,30 +1382,39 @@
       <c r="F15" t="inlineStr">
         <is>
           <t>&lt;p&gt;Consider the plot shown below, which shows the populations of North and South Korea from 1995 to 2013:&lt;/p&gt;
-&lt;pre class="r"&gt;&lt;code&gt;koreas_pop &amp;lt;-
-  tidyr::population %&amp;gt;% 
-  filter(country %in% c("Republic of Korea", 
-                        "Democratic People's Republic of Korea"))
-ggplot(data = koreas_pop,
-       mapping = aes(x = year, y = population, color = country)) + 
+&lt;pre class="r"&gt;&lt;code&gt;koreas_pop &amp;lt;-_x000D_
+  tidyr::population %&amp;gt;% _x000D_
+  filter(country %in% c("Republic of Korea", _x000D_
+                        "Democratic People's Republic of Korea"))_x000D_
+_x000D_
+ggplot(data = koreas_pop,_x000D_
+       mapping = aes(x = year, y = population, color = country)) + _x000D_
   geom_line()&lt;/code&gt;&lt;/pre&gt;
-&lt;p&gt;&lt;img src="https://drive.google.com/uc?export=view&amp;amp;id=15nB0SfXaWp5a7at1Zi7BAPacRlVp7NA4" width="672"&gt;&lt;/p&gt;
-&lt;p&gt;How could we change the code to generate a plot with thicker lines?&lt;/p&gt;</t>
+&lt;p&gt;&lt;img src="https://drive.google.com/uc?export=view&amp;amp;id=1LfCoLh5dPD-yGqgUmVA15asTAE8vbTBZ" width="672"&gt;&lt;/p&gt;
+&lt;p&gt;How could we change the code to generate a plot with thicker lines?&lt;/p&gt;
+&lt;p&gt;&lt;strong&gt;Important note&lt;/strong&gt;: the latest version of {ggplot2} has added an aesthetic called &lt;code&gt;linewidth&lt;/code&gt; that will replace &lt;code&gt;size&lt;/code&gt; aesthetic for scaling the width of lines in line based geoms like &lt;code&gt;geom_line()&lt;/code&gt;. Unfortunately, Our lesson was written and recorded before release of {ggplot2} 3.6.0 on 04/11/2022. The &lt;code&gt;size&lt;/code&gt; will still work, but it is recommended to update all code to reflect the new aesthetic. We have updated the quizzes and lesson code, however the lesson video has not been updated yet. Apologies for any inconvenience._x000D_
+If you not updated {ggplot2} since then 04/11/2022, please reinstall the latest version by restarting you R session and then running &lt;code&gt;install.packages("ggplot2")&lt;/code&gt; in R. You can find out which version you have installed by running &lt;code&gt;packageVersion("ggplot2")&lt;/code&gt; or by looking at the “Packages” tab in RStudio.&lt;/p&gt;</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>Add &lt;code&gt;size = 3&lt;/code&gt; inside the &lt;code&gt;aes()&lt;/code&gt; function.</t>
+          <t>&lt;div id="a-13" class="section level2"&gt;_x000D_
+&lt;h2&gt;A&lt;/h2&gt;_x000D_
+&lt;p&gt;Add &lt;code&gt;linewidth = 3&lt;/code&gt; inside the &lt;code&gt;aes()&lt;/code&gt; function.&lt;/p&gt;_x000D_&lt;/div&gt;</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>Add &lt;code&gt;size = 3&lt;/code&gt; inside the &lt;code&gt;geom_line()&lt;/code&gt; function.</t>
+          <t>&lt;div id="b-13" class="section level2"&gt;_x000D_
+&lt;h2&gt;B&lt;/h2&gt;_x000D_
+&lt;p&gt;Add &lt;code&gt;linewidth = 3&lt;/code&gt; inside the &lt;code&gt;geom_line()&lt;/code&gt; function.&lt;/p&gt;_x000D_&lt;/div&gt;</t>
         </is>
       </c>
       <c r="I15" t="inlineStr">
         <is>
-          <t>Add &lt;code&gt;size = 3&lt;/code&gt; inside the &lt;code&gt;ggplot()&lt;/code&gt; function, but outside the &lt;code&gt;aes()&lt;/code&gt; function.</t>
+          <t>&lt;div id="c-10" class="section level2"&gt;_x000D_
+&lt;h2&gt;C&lt;/h2&gt;_x000D_
+&lt;p&gt;Add &lt;code&gt;linewidth = 3&lt;/code&gt; inside the &lt;code&gt;ggplot()&lt;/code&gt; function, but outside the &lt;code&gt;aes()&lt;/code&gt; function.&lt;/p&gt;_x000D_&lt;/div&gt;</t>
         </is>
       </c>
       <c r="T15">
@@ -1283,25 +1422,29 @@
       </c>
       <c r="U15" t="inlineStr">
         <is>
-          <t>Great work! This is an example of &lt;em&gt;fixing&lt;/em&gt; an aesthetic (in this case, we want to fix the &lt;em&gt;size&lt;/em&gt; aesthetic of the lines to size &lt;code&gt;3&lt;/code&gt;).&lt;/p&gt;
-&lt;p&gt;Fixing an aesthetic should be done within the &lt;code&gt;geom_*&lt;/code&gt; function.&lt;/p&gt;
-&lt;p&gt;Here is the modified plot:&lt;/p&gt;
-&lt;pre class="r"&gt;&lt;code&gt;ggplot(data = koreas_pop,
-       mapping = aes(x = year, y = population, color = country)) + 
-  geom_line(size = 3)&lt;/code&gt;&lt;/pre&gt;
-&lt;p&gt;&lt;img src="https://drive.google.com/uc?export=view&amp;amp;id=1AuWQTGYI9wU8E4aVagDSiF5EhO7KElqw" width="672"&gt;&lt;/p&gt;
-&lt;p&gt;Remember that you can work with this dataset on your own computer; the &lt;code&gt;population&lt;/code&gt; dataset is loaded with the {tidyverse} packages.</t>
+          <t>&lt;div id="correct-message-13" class="section level2"&gt;_x000D_
+&lt;h2&gt;Correct message&lt;/h2&gt;_x000D_
+&lt;p&gt;Great work! This is an example of &lt;em&gt;fixing&lt;/em&gt; an aesthetic (in this case, we want to fix the &lt;code&gt;linewidth&lt;/code&gt; aesthetic of the lines to &lt;code&gt;3&lt;/code&gt;).&lt;/p&gt;_x000D_
+&lt;p&gt;Fixing an aesthetic should be done within the &lt;code&gt;geom_*&lt;/code&gt; function.&lt;/p&gt;_x000D_
+&lt;p&gt;Here is the modified plot:&lt;/p&gt;_x000D_
+&lt;pre class="r"&gt;&lt;code&gt;ggplot(data = koreas_pop,_x000D_
+       mapping = aes(x = year, y = population, color = country)) + _x000D_
+  geom_line(linewidth = 3)&lt;/code&gt;&lt;/pre&gt;_x000D_
+&lt;p&gt;&lt;img src="https://drive.google.com/uc?export=view&amp;amp;id=1FdPCCNfke_SX3t16TviqlS_3BaWhhNmR" width="672"&gt;&lt;/p&gt;_x000D_
+&lt;p&gt;Remember that you can work with this dataset on your own computer; the &lt;code&gt;population&lt;/code&gt; dataset is loaded with the {tidyverse} packages.&lt;/p&gt;_x000D_&lt;/div&gt;</t>
         </is>
       </c>
       <c r="V15" t="inlineStr">
         <is>
-          <t>This is an example of &lt;em&gt;fixing&lt;/em&gt; an aesthetic (in this case, we want to fix the &lt;em&gt;size&lt;/em&gt; aesthetic of the lines to size &lt;code&gt;3&lt;/code&gt;).&lt;/p&gt;
-&lt;p&gt;Fixing an aesthetic should be done within the &lt;code&gt;geom_*&lt;/code&gt; function.&lt;/p&gt;
-&lt;pre class="r"&gt;&lt;code&gt;ggplot(data = koreas_pop,
-       mapping = aes(x = year, y = population, color = country)) + 
-  geom_line(size = 3)&lt;/code&gt;&lt;/pre&gt;
-&lt;p&gt;&lt;img src="https://drive.google.com/uc?export=view&amp;amp;id=1EvCBB-iQLiPecPtyqjtLEJNLYHUy5HIX" width="672"&gt;&lt;/p&gt;
-&lt;p&gt;Remember that you can work with this dataset on your own computer; the &lt;code&gt;population&lt;/code&gt; dataset is loaded with the {tidyverse} packages.</t>
+          <t>&lt;div id="incorrect-message-13" class="section level2"&gt;_x000D_
+&lt;h2&gt;Incorrect message&lt;/h2&gt;_x000D_
+&lt;p&gt;This is an example of &lt;em&gt;fixing&lt;/em&gt; an aesthetic (in this case, we want to fix the &lt;code&gt;linewidth&lt;/code&gt; aesthetic of the lines to &lt;code&gt;3&lt;/code&gt;).&lt;/p&gt;_x000D_
+&lt;p&gt;Fixing an aesthetic should be done within the &lt;code&gt;geom_*&lt;/code&gt; function.&lt;/p&gt;_x000D_
+&lt;pre class="r"&gt;&lt;code&gt;ggplot(data = koreas_pop,_x000D_
+       mapping = aes(x = year, y = population, color = country)) + _x000D_
+  geom_line(linewidth = 3)&lt;/code&gt;&lt;/pre&gt;_x000D_
+&lt;p&gt;&lt;img src="https://drive.google.com/uc?export=view&amp;amp;id=1bDXjB3CeDz5TUJxUuot9rXsMcYWLXBss" width="672"&gt;&lt;/p&gt;_x000D_
+&lt;p&gt;Remember that you can work with this dataset on your own computer; the &lt;code&gt;population&lt;/code&gt; dataset is loaded with the {tidyverse} packages.&lt;/p&gt;_x000D_&lt;/div&gt;</t>
         </is>
       </c>
     </row>
@@ -1326,22 +1469,30 @@
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>&lt;code&gt;geom_col()&lt;/code&gt;</t>
+          <t>&lt;div id="a-14" class="section level2"&gt;_x000D_
+&lt;h2&gt;A&lt;/h2&gt;_x000D_
+&lt;p&gt;&lt;code&gt;geom_col()&lt;/code&gt;&lt;/p&gt;_x000D_&lt;/div&gt;</t>
         </is>
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>&lt;code&gt;geom_line()&lt;/code&gt;</t>
+          <t>&lt;div id="b-14" class="section level2"&gt;_x000D_
+&lt;h2&gt;B&lt;/h2&gt;_x000D_
+&lt;p&gt;&lt;code&gt;geom_line()&lt;/code&gt;&lt;/p&gt;_x000D_&lt;/div&gt;</t>
         </is>
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>&lt;code&gt;geom_point()&lt;/code&gt;</t>
+          <t>&lt;div id="c-11" class="section level2"&gt;_x000D_
+&lt;h2&gt;C&lt;/h2&gt;_x000D_
+&lt;p&gt;&lt;code&gt;geom_point()&lt;/code&gt;&lt;/p&gt;_x000D_&lt;/div&gt;</t>
         </is>
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>&lt;code&gt;geom_shade()&lt;/code&gt;</t>
+          <t>&lt;div id="d-4" class="section level2"&gt;_x000D_
+&lt;h2&gt;D&lt;/h2&gt;_x000D_
+&lt;p&gt;&lt;code&gt;geom_shade()&lt;/code&gt;&lt;/p&gt;_x000D_&lt;/div&gt;</t>
         </is>
       </c>
       <c r="T16">
@@ -1349,32 +1500,42 @@
       </c>
       <c r="U16" t="inlineStr">
         <is>
-          <t>That’s the one!&lt;/p&gt;
-&lt;p&gt;All others are valid (and very common) geoms.&lt;/p&gt;
-&lt;p&gt;Here is a plot with all three geoms, using the &lt;code&gt;population&lt;/code&gt; dataset from {tidyr}:&lt;/p&gt;
-&lt;pre class="r"&gt;&lt;code&gt;china_pop &amp;lt;- tidyr::population %&amp;gt;% filter(country == "China")
-ggplot(data = china_pop, 
-       mapping = aes(x = year, y = population)) + 
-  geom_col() + 
-  geom_point(size = 4) + 
-  geom_line(size = 2)&lt;/code&gt;&lt;/pre&gt;
-&lt;p&gt;&lt;img src="https://drive.google.com/uc?export=view&amp;amp;id=11-h0MgQRr9Vdlvp3-XMEUj52pFR0lMmr" width="672"&gt;&lt;/p&gt;
-&lt;p&gt;Of course, this is a &lt;em&gt;redundant&lt;/em&gt; plot. We don’t need three layers just to show one series of values. Only one of these geoms would be sufficient.</t>
+          <t>&lt;div id="correct-message-14" class="section level2"&gt;_x000D_
+&lt;h2&gt;Correct message&lt;/h2&gt;_x000D_
+&lt;p&gt;That’s the one!&lt;/p&gt;_x000D_
+&lt;p&gt;All others are valid (and very common) geoms.&lt;/p&gt;_x000D_
+&lt;p&gt;Here is a plot with all three geoms, using the &lt;code&gt;population&lt;/code&gt; dataset from {tidyr}:&lt;/p&gt;_x000D_
+&lt;pre class="r"&gt;&lt;code&gt;china_pop &amp;lt;- tidyr::population %&amp;gt;% filter(country == "China")_x000D_
+_x000D_
+ggplot(data = china_pop, _x000D_
+       mapping = aes(x = year, y = population)) + _x000D_
+  geom_col() + _x000D_
+  geom_point(size = 4) + _x000D_
+  geom_line(linewidth = 2)&lt;/code&gt;&lt;/pre&gt;_x000D_
+&lt;p&gt;&lt;img src="https://drive.google.com/uc?export=view&amp;amp;id=1uHFMYrsLLKlJ9F6FnfjLGFY9LW6lujFu" width="672"&gt;&lt;/p&gt;_x000D_
+&lt;p&gt;Of course, this is a &lt;em&gt;redundant&lt;/em&gt; plot. We don’t need three layers just to show one series of values. Only one of these geoms would be sufficient.&lt;/p&gt;_x000D_
+&lt;p&gt;&lt;strong&gt;Important note&lt;/strong&gt;: the latest version of {ggplot2} has added an aesthetic called &lt;code&gt;linewidth&lt;/code&gt; that will replace &lt;code&gt;size&lt;/code&gt; aesthetic for scaling the width of lines in line based geoms like &lt;code&gt;geom_line()&lt;/code&gt;. Unfortunately, Our lesson was written and recorded before release of {ggplot2} 3.6.0 on 04/11/2022. The &lt;code&gt;size&lt;/code&gt; will still work, but it is recommended to update all code to reflect the new aesthetic. We have updated the quizzes and lesson code, however the lesson video has not been updated yet. Apologies for any inconvenience._x000D_
+If you not updated {ggplot2} since then 04/11/2022, please reinstall the latest version by restarting you R session and then running &lt;code&gt;install.packages("ggplot2")&lt;/code&gt; in R. You can find out which version you have installed by running &lt;code&gt;packageVersion("ggplot2")&lt;/code&gt; or by looking at the “Packages” tab in RStudio.&lt;/p&gt;_x000D_&lt;/div&gt;</t>
         </is>
       </c>
       <c r="V16" t="inlineStr">
         <is>
-          <t>&lt;code&gt;geom_shade()&lt;/code&gt; is not a {ggplot2} function.&lt;/p&gt;
-&lt;p&gt;All others are valid (and very common) geoms.&lt;/p&gt;
-&lt;p&gt;Here is a plot with all three geoms, using the &lt;code&gt;population&lt;/code&gt; dataset from {tidyr}:&lt;/p&gt;
-&lt;pre class="r"&gt;&lt;code&gt;china_pop &amp;lt;- tidyr::population %&amp;gt;% filter(country == "China")
-ggplot(data = china_pop, 
-       mapping = aes(x = year, y = population)) + 
-  geom_col() + 
-  geom_point(size = 4) + 
-  geom_line(size = 2)&lt;/code&gt;&lt;/pre&gt;
-&lt;p&gt;&lt;img src="https://drive.google.com/uc?export=view&amp;amp;id=1ysaLAU2-u8pftZKGL3M0qTImdS_25eQn" width="672"&gt;&lt;/p&gt;
-&lt;p&gt;Of course, this is a &lt;em&gt;redundant&lt;/em&gt; plot. We don’t need three layers just to show one series of values. Only one of these geoms would be sufficient.</t>
+          <t>&lt;div id="incorrect-message-14" class="section level2"&gt;_x000D_
+&lt;h2&gt;Incorrect message&lt;/h2&gt;_x000D_
+&lt;p&gt;&lt;code&gt;geom_shade()&lt;/code&gt; is not a {ggplot2} function.&lt;/p&gt;_x000D_
+&lt;p&gt;All others are valid (and very common) geoms.&lt;/p&gt;_x000D_
+&lt;p&gt;Here is a plot with all three geoms, using the &lt;code&gt;population&lt;/code&gt; dataset from {tidyr}:&lt;/p&gt;_x000D_
+&lt;pre class="r"&gt;&lt;code&gt;china_pop &amp;lt;- tidyr::population %&amp;gt;% filter(country == "China")_x000D_
+_x000D_
+ggplot(data = china_pop, _x000D_
+       mapping = aes(x = year, y = population)) + _x000D_
+  geom_col() + _x000D_
+  geom_point(size = 4) + _x000D_
+  geom_line(linewidth = 2)&lt;/code&gt;&lt;/pre&gt;_x000D_
+&lt;p&gt;&lt;img src="https://drive.google.com/uc?export=view&amp;amp;id=10MR88ZabJLBZwzaQedpfCFXS1aEkupx1" width="672"&gt;&lt;/p&gt;_x000D_
+&lt;p&gt;Of course, this is a &lt;em&gt;redundant&lt;/em&gt; plot. We don’t need three layers just to show one series of values. Only one of these geoms would be sufficient.&lt;/p&gt;_x000D_
+&lt;p&gt;&lt;strong&gt;Important note&lt;/strong&gt;: the latest version of {ggplot2} has added an aesthetic called &lt;code&gt;linewidth&lt;/code&gt; that will replace &lt;code&gt;size&lt;/code&gt; aesthetic for scaling the width of lines in line based geoms like &lt;code&gt;geom_line()&lt;/code&gt;. Unfortunately, Our lesson was written and recorded before release of {ggplot2} 3.6.0 on 04/11/2022. The &lt;code&gt;size&lt;/code&gt; will still work, but it is recommended to update all code to reflect the new aesthetic. We have updated the quizzes and lesson code, however the lesson video has not been updated yet. Apologies for any inconvenience._x000D_
+If you not updated {ggplot2} since then 04/11/2022, please reinstall the latest version by restarting you R session and then running &lt;code&gt;install.packages("ggplot2")&lt;/code&gt; in R. You can find out which version you have installed by running &lt;code&gt;packageVersion("ggplot2")&lt;/code&gt; or by looking at the “Packages” tab in RStudio.&lt;/p&gt;_x000D_&lt;/div&gt;</t>
         </is>
       </c>
     </row>
@@ -1399,17 +1560,23 @@
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>&lt;code&gt;geom_scatterplot()&lt;/code&gt;</t>
+          <t>&lt;div id="a-15" class="section level2"&gt;_x000D_
+&lt;h2&gt;A&lt;/h2&gt;_x000D_
+&lt;p&gt;&lt;code&gt;geom_scatterplot()&lt;/code&gt;&lt;/p&gt;_x000D_&lt;/div&gt;</t>
         </is>
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>&lt;code&gt;geom_point()&lt;/code&gt;</t>
+          <t>&lt;div id="b-15" class="section level2"&gt;_x000D_
+&lt;h2&gt;B&lt;/h2&gt;_x000D_
+&lt;p&gt;&lt;code&gt;geom_point()&lt;/code&gt;&lt;/p&gt;_x000D_&lt;/div&gt;</t>
         </is>
       </c>
       <c r="I17" t="inlineStr">
         <is>
-          <t>&lt;code&gt;geom_line()&lt;/code&gt;</t>
+          <t>&lt;div id="c-12" class="section level2"&gt;_x000D_
+&lt;h2&gt;C&lt;/h2&gt;_x000D_
+&lt;p&gt;&lt;code&gt;geom_line()&lt;/code&gt;&lt;/p&gt;_x000D_&lt;/div&gt;</t>
         </is>
       </c>
       <c r="T17">
@@ -1417,25 +1584,29 @@
       </c>
       <c r="U17" t="inlineStr">
         <is>
-          <t>Great going!&lt;/p&gt;
-&lt;p&gt;&lt;code&gt;geom_scatterplot()&lt;/code&gt; is not a ggplot2 function. Scatter plots are typically created with &lt;code&gt;geom_point()&lt;/code&gt; in R. For example, here is a scatter plot of petal length and width in the &lt;code&gt;iris&lt;/code&gt; dataset, made with &lt;code&gt;geom_point()&lt;/code&gt;:&lt;/p&gt;
-&lt;pre class="r"&gt;&lt;code&gt;ggplot(iris, 
-       aes(x = Petal.Length, 
-           y = Petal.Width, 
-           color = Species)) + 
-  geom_point()&lt;/code&gt;&lt;/pre&gt;
-&lt;p&gt;&lt;img src="https://drive.google.com/uc?export=view&amp;amp;id=1fwGqjb3S4xUxqLzHZY7Oe4mwLOOslZjW" width="672"&gt;</t>
+          <t>&lt;div id="correct-message-15" class="section level2"&gt;_x000D_
+&lt;h2&gt;Correct message&lt;/h2&gt;_x000D_
+&lt;p&gt;Great going!&lt;/p&gt;_x000D_
+&lt;p&gt;&lt;code&gt;geom_scatterplot()&lt;/code&gt; is not a ggplot2 function. Scatter plots are typically created with &lt;code&gt;geom_point()&lt;/code&gt; in R. For example, here is a scatter plot of petal length and width in the &lt;code&gt;iris&lt;/code&gt; dataset, made with &lt;code&gt;geom_point()&lt;/code&gt;:&lt;/p&gt;_x000D_
+&lt;pre class="r"&gt;&lt;code&gt;ggplot(iris, _x000D_
+       aes(x = Petal.Length, _x000D_
+           y = Petal.Width, _x000D_
+           color = Species)) + _x000D_
+  geom_point()&lt;/code&gt;&lt;/pre&gt;_x000D_
+&lt;p&gt;&lt;img src="https://drive.google.com/uc?export=view&amp;amp;id=1zWFA_P1db8FlVuO2KgXfeXnM4jD7a8Mo" width="672"&gt;&lt;/p&gt;_x000D_&lt;/div&gt;</t>
         </is>
       </c>
       <c r="V17" t="inlineStr">
         <is>
-          <t>&lt;code&gt;geom_scatterplot()&lt;/code&gt; is not a ggplot2 function. Scatter plots are typically created with &lt;code&gt;geom_point()&lt;/code&gt; in R. For example, here is a scatter plot of petal length and width in the &lt;code&gt;iris&lt;/code&gt; dataset, made with &lt;code&gt;geom_point()&lt;/code&gt;:&lt;/p&gt;
-&lt;pre class="r"&gt;&lt;code&gt;ggplot(iris, 
-       aes(x = Petal.Length, 
-           y = Petal.Width, 
-           color = Species)) + 
-  geom_point()&lt;/code&gt;&lt;/pre&gt;
-&lt;p&gt;&lt;img src="https://drive.google.com/uc?export=view&amp;amp;id=1rHCpSpYTteSGzDMy69Ff7yGJ2uj14TFx" width="672"&gt;</t>
+          <t>&lt;div id="incorrect-message-15" class="section level2"&gt;_x000D_
+&lt;h2&gt;Incorrect message&lt;/h2&gt;_x000D_
+&lt;p&gt;&lt;code&gt;geom_scatterplot()&lt;/code&gt; is not a ggplot2 function. Scatter plots are typically created with &lt;code&gt;geom_point()&lt;/code&gt; in R. For example, here is a scatter plot of petal length and width in the &lt;code&gt;iris&lt;/code&gt; dataset, made with &lt;code&gt;geom_point()&lt;/code&gt;:&lt;/p&gt;_x000D_
+&lt;pre class="r"&gt;&lt;code&gt;ggplot(iris, _x000D_
+       aes(x = Petal.Length, _x000D_
+           y = Petal.Width, _x000D_
+           color = Species)) + _x000D_
+  geom_point()&lt;/code&gt;&lt;/pre&gt;_x000D_
+&lt;p&gt;&lt;img src="https://drive.google.com/uc?export=view&amp;amp;id=1TRcs0VlB3scHebuvf5RFJWr0TcPSVcFq" width="672"&gt;&lt;/p&gt;_x000D_&lt;/div&gt;</t>
         </is>
       </c>
     </row>
@@ -1456,50 +1627,59 @@
       <c r="F18" t="inlineStr">
         <is>
           <t>&lt;p&gt;The following code chunk generates a scatterplot of age and the daily number of TV hours watched, from a survey in the US:&lt;/p&gt;
-&lt;pre class="r"&gt;&lt;code&gt;survey_sample &amp;lt;- forcats::gss_cat %&amp;gt;% slice_sample(n = 200) # sample 100 respondents
+&lt;pre class="r"&gt;&lt;code&gt;survey_sample &amp;lt;- forcats::gss_cat %&amp;gt;% slice_sample(n = 200) # sample 200 respondents_x000D_
 head(survey_sample)&lt;/code&gt;&lt;/pre&gt;
-&lt;pre&gt;&lt;code&gt;## # A tibble: 6 × 9
-##    year marital         age race  rincome        partyid    relig denom tvhours
-##   &amp;lt;int&amp;gt; &amp;lt;fct&amp;gt;         &amp;lt;int&amp;gt; &amp;lt;fct&amp;gt; &amp;lt;fct&amp;gt;          &amp;lt;fct&amp;gt;      &amp;lt;fct&amp;gt; &amp;lt;fct&amp;gt;   &amp;lt;int&amp;gt;
-## 1  2000 Widowed          73 White Not applicable Not str r… Prot… Bapt…       2
-## 2  2002 Never married    32 Black $25000 or more Strong de… Inte… Not …      NA
-## 3  2014 Married          35 White Not applicable Independe… Prot… Other       1
-## 4  2004 Married          57 Other $25000 or more Not str d… Cath… Not …      NA
-## 5  2006 Never married    36 White $15000 - 19999 Ind,near … Prot… Other      NA
-## 6  2010 Divorced         38 White $25000 or more Not str d… Cath… Not …      NA&lt;/code&gt;&lt;/pre&gt;
-&lt;pre class="r"&gt;&lt;code&gt;ggplot(survey_sample, 
-       aes(x = age, y = tvhours)) + 
+&lt;pre&gt;&lt;code&gt;## # A tibble: 6 × 9_x000D_
+##    year marital   age race  rincome partyid relig denom_x000D_
+##   &amp;lt;int&amp;gt; &amp;lt;fct&amp;gt;   &amp;lt;int&amp;gt; &amp;lt;fct&amp;gt; &amp;lt;fct&amp;gt;   &amp;lt;fct&amp;gt;   &amp;lt;fct&amp;gt; &amp;lt;fct&amp;gt;_x000D_
+## 1  2002 Separa…    33 White $15000… Not st… Chri… Not …_x000D_
+## 2  2006 Divorc…    57 Black Not ap… Strong… Prot… Sout…_x000D_
+## 3  2008 Married    28 White $25000… Not st… Prot… Sout…_x000D_
+## 4  2002 Never …    29 White $25000… Strong… Cath… Not …_x000D_
+## 5  2006 Separa…    75 White Not ap… Ind,ne… Cath… Not …_x000D_
+## 6  2000 Married    32 Other $20000… Indepe… Cath… Not …_x000D_
+## # … with 1 more variable: tvhours &amp;lt;int&amp;gt;&lt;/code&gt;&lt;/pre&gt;
+&lt;pre class="r"&gt;&lt;code&gt;ggplot(survey_sample, _x000D_
+       aes(x = age, y = tvhours)) + _x000D_
   geom_point()&lt;/code&gt;&lt;/pre&gt;
-&lt;p&gt;&lt;img src="https://drive.google.com/uc?export=view&amp;amp;id=1ijG-mTeuB-9IXO8P5h0kMJphaK39waCx" width="672"&gt;&lt;/p&gt;
+&lt;p&gt;&lt;img src="https://drive.google.com/uc?export=view&amp;amp;id=1AgAEP2S7iKA0UTMmqdMgJ8gEoiDg-SQ0" width="672"&gt;&lt;/p&gt;
 &lt;p&gt;Which of the following would apply an aesthetic mapping to differentiate by the &lt;code&gt;marital&lt;/code&gt; variable?&lt;/p&gt;</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>&lt;div id="a-16" class="section level2"&gt;&lt;pre class="r"&gt;&lt;code&gt;ggplot(survey_sample,
-       aes(x = age, y = tvhours)) + 
-  geom_point(color = marital)&lt;/code&gt;&lt;/pre&gt;&lt;/div&gt;</t>
+          <t>&lt;div id="a-16" class="section level2"&gt;_x000D_
+&lt;h2&gt;A&lt;/h2&gt;_x000D_
+&lt;pre class="r"&gt;&lt;code&gt;ggplot(survey_sample,_x000D_
+       aes(x = age, y = tvhours)) + _x000D_
+  geom_point(color = marital)&lt;/code&gt;&lt;/pre&gt;_x000D_&lt;/div&gt;</t>
         </is>
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>&lt;div id="b-16" class="section level2"&gt;&lt;pre class="r"&gt;&lt;code&gt;ggplot(survey_sample,
-       aes(x = age, y = tvhours)) + 
-  geom_point_colored(color = marital)&lt;/code&gt;&lt;/pre&gt;&lt;/div&gt;</t>
+          <t>&lt;div id="b-16" class="section level2"&gt;_x000D_
+&lt;h2&gt;B&lt;/h2&gt;_x000D_
+&lt;pre class="r"&gt;&lt;code&gt;ggplot(survey_sample,_x000D_
+       aes(x = age, y = tvhours)) + _x000D_
+  geom_point_colored(color = marital)&lt;/code&gt;&lt;/pre&gt;_x000D_&lt;/div&gt;</t>
         </is>
       </c>
       <c r="I18" t="inlineStr">
         <is>
-          <t>&lt;div id="c-13" class="section level2"&gt;&lt;pre class="r"&gt;&lt;code&gt;ggplot(survey_sample,
-       aes(x = age, y = tvhours, color = marital)) + 
-  geom_point()&lt;/code&gt;&lt;/pre&gt;&lt;/div&gt;</t>
+          <t>&lt;div id="c-13" class="section level2"&gt;_x000D_
+&lt;h2&gt;C&lt;/h2&gt;_x000D_
+&lt;pre class="r"&gt;&lt;code&gt;ggplot(survey_sample,_x000D_
+       aes(x = age, y = tvhours, color = marital)) + _x000D_
+  geom_point()&lt;/code&gt;&lt;/pre&gt;_x000D_&lt;/div&gt;</t>
         </is>
       </c>
       <c r="J18" t="inlineStr">
         <is>
-          <t>&lt;div id="d-5" class="section level2"&gt;&lt;pre class="r"&gt;&lt;code&gt;ggplot(survey_sample,
-       aes(x = age, y = bmi)) + 
-  geom_point(sex = c(male = "blue", female = "orange"))&lt;/code&gt;&lt;/pre&gt;&lt;/div&gt;</t>
+          <t>&lt;div id="d-5" class="section level2"&gt;_x000D_
+&lt;h2&gt;D&lt;/h2&gt;_x000D_
+&lt;pre class="r"&gt;&lt;code&gt;ggplot(survey_sample,_x000D_
+       aes(x = age, y = bmi)) + _x000D_
+  geom_point(sex = c(male = "blue", female = "orange"))&lt;/code&gt;&lt;/pre&gt;_x000D_&lt;/div&gt;</t>
         </is>
       </c>
       <c r="T18">
@@ -1507,25 +1687,136 @@
       </c>
       <c r="U18" t="inlineStr">
         <is>
-          <t>You got it!&lt;/p&gt;
-&lt;p&gt;&lt;code&gt;color = marital&lt;/code&gt; inside the &lt;code&gt;aes&lt;/code&gt; mapping will produce different colors for each marital status. The other three code chunks don’t work.&lt;/p&gt;
-&lt;p&gt;Here is the final plot:&lt;/p&gt;
-&lt;pre class="r"&gt;&lt;code&gt;ggplot(survey_sample,
-       aes(x = age, y = tvhours, color = marital)) + 
-  geom_point()&lt;/code&gt;&lt;/pre&gt;
-&lt;p&gt;&lt;img src="https://drive.google.com/uc?export=view&amp;amp;id=1f6aU9VSdAZxtwruLUC61NKBBOmzPF6ww" width="672"&gt;&lt;/p&gt;
-&lt;p&gt;The {forcats} package is part of the tidyverse, so you should be able to work with this data on your own computer</t>
+          <t>&lt;div id="correct-message-16" class="section level2"&gt;_x000D_
+&lt;h2&gt;Correct message&lt;/h2&gt;_x000D_
+&lt;p&gt;You got it!&lt;/p&gt;_x000D_
+&lt;p&gt;&lt;code&gt;color = marital&lt;/code&gt; inside the &lt;code&gt;aes&lt;/code&gt; mapping will produce different colors for each marital status. The other three code chunks don’t work.&lt;/p&gt;_x000D_
+&lt;p&gt;Here is the final plot:&lt;/p&gt;_x000D_
+&lt;pre class="r"&gt;&lt;code&gt;ggplot(survey_sample,_x000D_
+       aes(x = age, y = tvhours, color = marital)) + _x000D_
+  geom_point()&lt;/code&gt;&lt;/pre&gt;_x000D_
+&lt;p&gt;&lt;img src="https://drive.google.com/uc?export=view&amp;amp;id=19Vj30V_Gq_-T1jZW5gNFd19_NOPbLqn9" width="672"&gt;&lt;/p&gt;_x000D_
+&lt;p&gt;The {forcats} package is part of the tidyverse, so you should be able to work with this data on your own computer&lt;/p&gt;_x000D_&lt;/div&gt;</t>
         </is>
       </c>
       <c r="V18" t="inlineStr">
         <is>
-          <t>&lt;code&gt;color = marital&lt;/code&gt; inside the &lt;code&gt;aes&lt;/code&gt; mapping will produce different colors for each marital status. The other three code chunks don’t work.&lt;/p&gt;
-&lt;p&gt;Here is the final plot:&lt;/p&gt;
-&lt;pre class="r"&gt;&lt;code&gt;ggplot(survey_sample,
-       aes(x = age, y = tvhours, color = marital)) + 
-  geom_point()&lt;/code&gt;&lt;/pre&gt;
-&lt;p&gt;&lt;img src="https://drive.google.com/uc?export=view&amp;amp;id=1vvPdMnKTnDem7N35EosYU7DTdbYPEoKe" width="672"&gt;&lt;/p&gt;
-&lt;p&gt;The {forcats} package is part of the tidyverse, so you should be able to work with this data on your own computer</t>
+          <t>&lt;div id="incorrect-message-16" class="section level2"&gt;_x000D_
+&lt;h2&gt;Incorrect message&lt;/h2&gt;_x000D_
+&lt;p&gt;&lt;code&gt;color = marital&lt;/code&gt; inside the &lt;code&gt;aes&lt;/code&gt; mapping will produce different colors for each marital status. The other three code chunks don’t work.&lt;/p&gt;_x000D_
+&lt;p&gt;Here is the final plot:&lt;/p&gt;_x000D_
+&lt;pre class="r"&gt;&lt;code&gt;ggplot(survey_sample,_x000D_
+       aes(x = age, y = tvhours, color = marital)) + _x000D_
+  geom_point()&lt;/code&gt;&lt;/pre&gt;_x000D_
+&lt;p&gt;&lt;img src="https://drive.google.com/uc?export=view&amp;amp;id=1mAUuJBGycxVnRoXYeg3Vl0DzuzAz2EsT" width="672"&gt;&lt;/p&gt;_x000D_
+&lt;p&gt;The {forcats} package is part of the tidyverse, so you should be able to work with this data on your own computer&lt;/p&gt;_x000D_&lt;/div&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>#q-27</t>
+        </is>
+      </c>
+      <c r="D19">
+        <v>1</v>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>single</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>&lt;p&gt;Take a look at the first 6 rows of this dataset, which records the total number of HIV cases per year in Ghana, Thailand, and Zambia from 1995 to 2009.&lt;/p&gt;
+&lt;pre class="r"&gt;&lt;code&gt;head(hiv_prevalence)&lt;/code&gt;&lt;/pre&gt;
+&lt;pre&gt;&lt;code&gt;## # A tibble: 6 × 4_x000D_
+##   country  year total_cases population_x000D_
+##   &amp;lt;chr&amp;gt;   &amp;lt;int&amp;gt;       &amp;lt;dbl&amp;gt;      &amp;lt;int&amp;gt;_x000D_
+## 1 Ghana    1995      170000   16760926_x000D_
+## 2 Ghana    1996      190000   17169151_x000D_
+## 3 Ghana    1997      200000   17568461_x000D_
+## 4 Ghana    1998      220000   17968830_x000D_
+## 5 Ghana    1999      230000   18384302_x000D_
+## 6 Ghana    2000      240000   18825034&lt;/code&gt;&lt;/pre&gt;
+&lt;p&gt;We plotted the following line graph showing &lt;code&gt;total_cases&lt;/code&gt; per &lt;code&gt;year&lt;/code&gt; using &lt;code&gt;geom_line()&lt;/code&gt;:&lt;/p&gt;
+&lt;p&gt;&lt;img src="https://drive.google.com/uc?export=view&amp;amp;id=1NktIwbVqA7hlep3V2rTITc-AncgVFtyJ" width="672"&gt;&lt;/p&gt;
+&lt;p&gt;All EXCEPT ONE of the following statements is true about the &lt;code&gt;ggplot&lt;/code&gt; code needed to create this plot.&lt;/p&gt;
+&lt;p&gt;Which statement is FALSE?&lt;/p&gt;</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>&lt;div id="a-17" class="section level2"&gt;_x000D_
+&lt;h2&gt;A&lt;/h2&gt;_x000D_
+&lt;p&gt;The &lt;code&gt;x&lt;/code&gt; aesthetic argument should go inside &lt;code&gt;aes()&lt;/code&gt;.&lt;/p&gt;_x000D_&lt;/div&gt;</t>
+        </is>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>&lt;div id="b-17" class="section level2"&gt;_x000D_
+&lt;h2&gt;B&lt;/h2&gt;_x000D_
+&lt;p&gt;The &lt;code&gt;y&lt;/code&gt; aesthetic argument should go inside &lt;code&gt;aes()&lt;/code&gt;.&lt;/p&gt;_x000D_&lt;/div&gt;</t>
+        </is>
+      </c>
+      <c r="I19" t="inlineStr">
+        <is>
+          <t>&lt;div id="c-14" class="section level2"&gt;_x000D_
+&lt;h2&gt;C&lt;/h2&gt;_x000D_
+&lt;p&gt;The &lt;code&gt;color&lt;/code&gt; aesthetic argument should go outside &lt;code&gt;aes()&lt;/code&gt;.&lt;/p&gt;_x000D_&lt;/div&gt;</t>
+        </is>
+      </c>
+      <c r="J19" t="inlineStr">
+        <is>
+          <t>&lt;div id="d-6" class="section level2"&gt;_x000D_
+&lt;h2&gt;D&lt;/h2&gt;_x000D_
+&lt;p&gt;The &lt;code&gt;color&lt;/code&gt; aesthetic argument should go inside &lt;code&gt;aes()&lt;/code&gt;.&lt;/p&gt;_x000D_&lt;/div&gt;</t>
+        </is>
+      </c>
+      <c r="T19">
+        <v>3</v>
+      </c>
+      <c r="U19" t="inlineStr">
+        <is>
+          <t>&lt;div id="correct-message-17" class="section level2"&gt;_x000D_
+&lt;h2&gt;Correct message&lt;/h2&gt;_x000D_
+&lt;p&gt;Great job!&lt;/p&gt;_x000D_
+&lt;p&gt;You can tell that color is an aesthetic &lt;strong&gt;mapping&lt;/strong&gt; and not a &lt;strong&gt;fixed&lt;/strong&gt; aesthetic because the lines in this plot are different for each country. Since the color of geoms is informed by a data variable, it must go in &lt;code&gt;mapping = aes()&lt;/code&gt;.&lt;/p&gt;_x000D_
+&lt;p&gt;Here is the code used to create this plot:&lt;/p&gt;_x000D_
+&lt;pre class="r"&gt;&lt;code&gt;ggplot(hiv_prevalence, _x000D_
+       mapping = aes(x = year, _x000D_
+                     y = total_cases, _x000D_
+                     color = country)) +_x000D_
+  geom_line()&lt;/code&gt;&lt;/pre&gt;_x000D_
+&lt;p&gt;&lt;strong&gt;&lt;code&gt;ggplot()&lt;/code&gt;&lt;/strong&gt; is &lt;strong&gt;&lt;code&gt;mapping&lt;/code&gt;&lt;/strong&gt; three data variables inside &lt;strong&gt;&lt;code&gt;aes()&lt;/code&gt;&lt;/strong&gt;:&lt;/p&gt;_x000D_
+&lt;ul&gt;
+&lt;li&gt;&lt;p&gt;&lt;code&gt;year&lt;/code&gt; is mapped to the &lt;code&gt;x&lt;/code&gt; position aesthetic&lt;/p&gt;&lt;/li&gt;_x000D_
+&lt;li&gt;&lt;p&gt;&lt;code&gt;total_cases&lt;/code&gt; is mapped to the &lt;code&gt;y&lt;/code&gt; position aesthetic&lt;/p&gt;&lt;/li&gt;_x000D_
+&lt;li&gt;&lt;p&gt;&lt;code&gt;country&lt;/code&gt; is mapped to the &lt;code&gt;color&lt;/code&gt; aesthetic.&lt;/p&gt;&lt;/li&gt;_x000D_
+&lt;/ul&gt;
+&lt;p&gt;If we want to set &lt;code&gt;color&lt;/code&gt; to a constant value like &lt;code&gt;"red"&lt;/code&gt; , it should outside &lt;code&gt;aes()&lt;/code&gt; as a fixed aesthetic.&lt;/p&gt;_x000D_&lt;/div&gt;</t>
+        </is>
+      </c>
+      <c r="V19" t="inlineStr">
+        <is>
+          <t>&lt;div id="incorrect-message-17" class="section level2"&gt;_x000D_
+&lt;h2&gt;Incorrect message&lt;/h2&gt;_x000D_
+&lt;p&gt;This question is testing your knowledge of how to use aesthetic mappings vs. fixed aesthetics.&lt;/p&gt;_x000D_
+&lt;p&gt;You can tell that color is an aesthetic &lt;strong&gt;mapping&lt;/strong&gt; and not a &lt;strong&gt;fixed&lt;/strong&gt; aesthetic because the lines in this plot are different for each country. Since the color of geoms is informed by a data variable, it must go in &lt;code&gt;mapping = aes()&lt;/code&gt;.&lt;/p&gt;_x000D_
+&lt;p&gt;Here is the code used to create this plot:&lt;/p&gt;_x000D_
+&lt;pre class="r"&gt;&lt;code&gt;ggplot(hiv_prevalence, _x000D_
+       mapping = aes(x = year, _x000D_
+                     y = total_cases, _x000D_
+                     color = country)) +_x000D_
+  geom_line()&lt;/code&gt;&lt;/pre&gt;_x000D_
+&lt;p&gt;&lt;strong&gt;&lt;code&gt;ggplot()&lt;/code&gt;&lt;/strong&gt; is &lt;strong&gt;&lt;code&gt;mapping&lt;/code&gt;&lt;/strong&gt; three data variables inside &lt;strong&gt;&lt;code&gt;aes()&lt;/code&gt;&lt;/strong&gt;:&lt;/p&gt;_x000D_
+&lt;ul&gt;
+&lt;li&gt;&lt;p&gt;&lt;code&gt;year&lt;/code&gt; is mapped to the &lt;code&gt;x&lt;/code&gt; position aesthetic&lt;/p&gt;&lt;/li&gt;_x000D_
+&lt;li&gt;&lt;p&gt;&lt;code&gt;total_cases&lt;/code&gt; is mapped to the &lt;code&gt;y&lt;/code&gt; position aesthetic&lt;/p&gt;&lt;/li&gt;_x000D_
+&lt;li&gt;&lt;p&gt;&lt;code&gt;country&lt;/code&gt; is mapped to the &lt;code&gt;color&lt;/code&gt; aesthetic.&lt;/p&gt;&lt;/li&gt;_x000D_
+&lt;/ul&gt;
+&lt;p&gt;If we want to set &lt;code&gt;color&lt;/code&gt; to a constant value like &lt;code&gt;"red"&lt;/code&gt; , it should outside &lt;code&gt;aes()&lt;/code&gt; as a fixed aesthetic.&lt;/p&gt;_x000D_&lt;/div&gt;</t>
         </is>
       </c>
     </row>

</xml_diff>